<commit_message>
Downloaded all the Datasheets
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -5,30 +5,41 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\SINDiB-MicroMouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\SINDiB-MICROMOUSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480F9C91-4228-457F-8205-58C69EDD4D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FF3538-F52A-4837-9967-500AADB6625A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
+    <workbookView xWindow="1620" yWindow="1395" windowWidth="21600" windowHeight="11295" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$H$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$H$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="81">
   <si>
     <t>COMPONENT</t>
   </si>
@@ -117,9 +128,6 @@
     <t>3.7V,  (Aliexpress - 5 - 400mAh with charger)</t>
   </si>
   <si>
-    <t>Tronic - RS. 30.00</t>
-  </si>
-  <si>
     <t>Extra</t>
   </si>
   <si>
@@ -153,9 +161,6 @@
     <t>Tronic.lk - RS.30.00</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Tronic.lk - RS. 20.00</t>
   </si>
   <si>
@@ -174,9 +179,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>10pF, 1.5nF, 0.1uF,  0.1uF(25V),  2.2uF, 4.7uF, 10uF</t>
-  </si>
-  <si>
     <t>Push Button</t>
   </si>
   <si>
@@ -201,9 +203,6 @@
     <t>220uF - 10V</t>
   </si>
   <si>
-    <t>0603: {1k,  10k, 47k, 20k}, 0805 : {10, 1.8k}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resistor Kit </t>
   </si>
   <si>
@@ -232,6 +231,57 @@
   </si>
   <si>
     <t>AMOUNT(LKR)</t>
+  </si>
+  <si>
+    <t>FDV303N</t>
+  </si>
+  <si>
+    <t>Tronic</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>1N4148W</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>OLED Display</t>
+  </si>
+  <si>
+    <t>128*64 --&gt; SPI Communication</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Slide Switch</t>
+  </si>
+  <si>
+    <t>N-Channel MOSFET (V_GS = 3.3V, I_DS = .1mA)</t>
+  </si>
+  <si>
+    <t>Fast Switching Diode</t>
+  </si>
+  <si>
+    <t>Debug Tool</t>
+  </si>
+  <si>
+    <t>0603: {1k,  10k, 43k, 20k}, 0805 : {10, 1.8k}</t>
+  </si>
+  <si>
+    <t>10pF, 1.5nF, 0.1uF,  0.01uF(25V),  2.2uF, 4.7uF, 10uF</t>
+  </si>
+  <si>
+    <t>CRO</t>
+  </si>
+  <si>
+    <t>16MHz</t>
   </si>
 </sst>
 </file>
@@ -286,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +373,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -428,7 +484,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -446,7 +502,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -458,15 +514,116 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -481,64 +638,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -548,24 +647,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -592,7 +679,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -602,33 +689,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -947,96 +1066,96 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:M33"/>
+  <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="66.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="18.109375" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="66.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+    </row>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="38" t="s">
+      <c r="F4" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="31">
+      <c r="K4" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="36">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="37">
         <v>2</v>
       </c>
-      <c r="F5" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="34">
+      <c r="F5" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="39">
         <v>7</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="23">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
         <v>2</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1044,48 +1163,48 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="20">
+        <v>49</v>
+      </c>
+      <c r="G6" s="16">
         <v>7.82</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="23">
+    <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="19">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="49" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="16">
+        <v>49</v>
+      </c>
+      <c r="G7" s="12">
         <v>40.67</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-    </row>
-    <row r="8" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31">
+      <c r="K7" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+    </row>
+    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36">
         <v>4</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1093,48 +1212,48 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="16">
+        <v>49</v>
+      </c>
+      <c r="G8" s="12">
         <v>9.2799999999999994</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="23">
+    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="19">
         <v>5</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="52"/>
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="14">
-        <v>1</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="25" t="s">
+      <c r="E9" s="10">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="L9" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="M9" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="23">
+    </row>
+    <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="19">
         <v>6</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1142,29 +1261,29 @@
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="16">
+        <v>49</v>
+      </c>
+      <c r="G10" s="12">
         <v>3.5</v>
       </c>
-      <c r="H10" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="L10" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M10" s="32">
+      <c r="H10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="23">
         <v>44809.72</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="31">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="36">
         <v>7</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="49" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1174,23 +1293,23 @@
         <v>1</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="16">
+        <v>49</v>
+      </c>
+      <c r="G11" s="12">
         <v>7.33</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="20" t="s">
         <v>15</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="23">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="19">
         <v>8</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1198,20 +1317,20 @@
         <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="16">
+        <v>49</v>
+      </c>
+      <c r="G12" s="12">
         <v>5.1100000000000003</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="23">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="19">
         <v>9</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1219,307 +1338,389 @@
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="16">
+        <v>49</v>
+      </c>
+      <c r="G13" s="12">
         <v>11.25</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="31">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="19">
+        <v>11</v>
+      </c>
+      <c r="C14" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="23">
-        <v>11</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="10" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="19">
+        <v>12</v>
+      </c>
+      <c r="C15" s="52"/>
+      <c r="D15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="23">
-        <v>12</v>
-      </c>
-      <c r="C16" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="36">
+        <v>13</v>
+      </c>
+      <c r="C16" s="52"/>
       <c r="D16" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="16">
+        <v>49</v>
+      </c>
+      <c r="G16" s="12">
         <v>3.92</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="19">
+        <v>14</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="2" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="31">
-        <v>13</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="16">
+        <v>49</v>
+      </c>
+      <c r="G17" s="12">
         <v>11.82</v>
       </c>
-      <c r="H17" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="23">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="H17" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="19">
+        <v>15</v>
+      </c>
+      <c r="C18" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="10">
+        <v>5</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="36">
+        <v>16</v>
+      </c>
+      <c r="C19" s="52"/>
+      <c r="D19" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="19">
+        <v>17</v>
+      </c>
+      <c r="C20" s="53"/>
+      <c r="D20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="19">
+        <v>18</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="47">
+        <v>5</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="36">
+        <v>19</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="25"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="23">
-        <v>15</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="24"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="31">
-        <v>16</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="24"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="23">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="14">
-        <v>5</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="23">
-        <v>18</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="12">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="16">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="31">
-        <v>19</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="14">
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="19">
+        <v>20</v>
+      </c>
+      <c r="C23" s="52"/>
+      <c r="D23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="10">
         <v>5</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="23">
-        <v>20</v>
-      </c>
-      <c r="C24" s="6"/>
+      <c r="F23" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="19">
+        <v>21</v>
+      </c>
+      <c r="C24" s="52"/>
       <c r="D24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="16">
+        <v>49</v>
+      </c>
+      <c r="G24" s="12">
         <v>17.489999999999998</v>
       </c>
-      <c r="H24" s="24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="23">
-        <v>21</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="14" t="s">
+      <c r="H24" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="36">
+        <v>22</v>
+      </c>
+      <c r="C25" s="52"/>
+      <c r="D25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="10">
+        <v>6</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="14">
-        <v>6</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="31">
-        <v>22</v>
-      </c>
-      <c r="C26" s="6"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="19">
+        <v>23</v>
+      </c>
+      <c r="C26" s="52"/>
       <c r="D26" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2">
         <v>2</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="16">
+        <v>49</v>
+      </c>
+      <c r="G26" s="12">
         <v>4.21</v>
       </c>
-      <c r="H26" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="23">
-        <v>23</v>
-      </c>
-      <c r="C27" s="7"/>
+      <c r="H26" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="19">
+        <v>24</v>
+      </c>
+      <c r="C27" s="52"/>
       <c r="D27" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="16">
+        <v>49</v>
+      </c>
+      <c r="G27" s="12">
         <v>0.49</v>
       </c>
-      <c r="H27" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="30"/>
-    </row>
-    <row r="29" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="22">
-        <f>SUM(G5:G27)</f>
+      <c r="H27" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="48"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="32">
+        <v>3</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="36">
+        <v>25</v>
+      </c>
+      <c r="C29" s="53"/>
+      <c r="D29" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="32">
+        <v>2</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="42"/>
+      <c r="H29" s="35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="19">
+        <v>26</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="32">
+        <v>10</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="34"/>
+      <c r="H30" s="35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="19">
+        <v>27</v>
+      </c>
+      <c r="C31" s="50"/>
+      <c r="D31" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="43">
+        <v>2</v>
+      </c>
+      <c r="F31" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="44"/>
+      <c r="H31" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" s="18">
+        <f>SUM(G5:G31)</f>
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C33" s="1" t="s">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="C21:C29"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C14:C17"/>
     <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{009E80E0-CC73-4407-97F9-5CA562932134}"/>
@@ -1539,8 +1740,12 @@
     <hyperlink ref="F24" r:id="rId15" xr:uid="{D53C4188-224B-4190-91FC-BDD4B0CE1088}"/>
     <hyperlink ref="F26" r:id="rId16" xr:uid="{2BDB80E1-F69C-4A65-BE00-E96747144E0E}"/>
     <hyperlink ref="F27" r:id="rId17" xr:uid="{A1216382-173D-4DE8-8B55-B8AA0B432E5E}"/>
+    <hyperlink ref="F30" r:id="rId18" xr:uid="{537B03B5-DE99-4376-A395-EA76E9416915}"/>
+    <hyperlink ref="F31" r:id="rId19" xr:uid="{A76581A8-80D9-4C32-A637-E5C30AC9CBF4}"/>
+    <hyperlink ref="F29" r:id="rId20" xr:uid="{F420E434-709D-4376-89CE-505F92CFCB33}"/>
+    <hyperlink ref="F28" r:id="rId21" xr:uid="{D9718443-4813-40E0-A6BD-4DB2D05599CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="62" orientation="landscape" r:id="rId18"/>
+  <pageSetup scale="62" orientation="landscape" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Finalized PCB Files & BOM Update
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\SINDiB-MICROMOUSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CBE6E4-09BA-4744-98D3-3B9D533FFDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D8307B-E79E-44A3-B8A0-95169180C92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$H$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$I$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
   <si>
     <t>COMPONENT</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Inductor - 0805</t>
   </si>
   <si>
-    <t>Tronic.lk - RS.30.00</t>
-  </si>
-  <si>
-    <t>Tronic.lk - RS. 20.00</t>
-  </si>
-  <si>
     <t>Capacitor - 1206</t>
   </si>
   <si>
@@ -194,9 +188,6 @@
     <t xml:space="preserve">3.3V Linear Regulator </t>
   </si>
   <si>
-    <t>FINAL PRICE (USD)</t>
-  </si>
-  <si>
     <t>HAVE</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>Sanjith</t>
   </si>
   <si>
-    <t>Aliexpress Order</t>
-  </si>
-  <si>
     <t>AMOUNT(LKR)</t>
   </si>
   <si>
@@ -242,9 +230,6 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>Slide Switch</t>
-  </si>
-  <si>
     <t>N-Channel MOSFET (V_GS = 3.3V, I_DS = .1mA)</t>
   </si>
   <si>
@@ -263,9 +248,6 @@
     <t>CRO</t>
   </si>
   <si>
-    <t>16MHz</t>
-  </si>
-  <si>
     <t>N20-Motor</t>
   </si>
   <si>
@@ -312,6 +294,54 @@
   </si>
   <si>
     <t>Low Drop Voltage - 3.3V Linear Regulator</t>
+  </si>
+  <si>
+    <t>3-SPDTT Slide Switch</t>
+  </si>
+  <si>
+    <t>6*6*7mm</t>
+  </si>
+  <si>
+    <t>Daraz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (USD)</t>
+  </si>
+  <si>
+    <t>(LKR)</t>
+  </si>
+  <si>
+    <t>Aliexpress Order - I</t>
+  </si>
+  <si>
+    <t>Aliexpress Order - II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reimbursement </t>
+  </si>
+  <si>
+    <t>Divakaran</t>
+  </si>
+  <si>
+    <t>N20-Mount</t>
+  </si>
+  <si>
+    <t>Monut for Motor</t>
+  </si>
+  <si>
+    <t>16MHz, 2Pin SMD</t>
+  </si>
+  <si>
+    <t>Chamith</t>
+  </si>
+  <si>
+    <t>Duino</t>
+  </si>
+  <si>
+    <t>PCB - JLCPCB</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -372,7 +402,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,12 +465,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -704,37 +758,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -753,41 +846,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -795,10 +865,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -822,8 +888,78 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -833,6 +969,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD28080"/>
+      <color rgb="FFFF6600"/>
       <color rgb="FFE2A49A"/>
     </mruColors>
   </colors>
@@ -1147,10 +1285,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M43"/>
+  <dimension ref="B1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,93 +1298,98 @@
     <col min="4" max="4" width="28" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="66.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="66.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="36" t="s">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="K2" s="60" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K3" s="61" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="L2" s="40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="21">
+        <v>1</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="K4" s="59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="33">
-        <v>1</v>
-      </c>
-      <c r="C5" s="35" t="s">
+      <c r="G5" s="27">
         <v>7</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="18">
+      <c r="H5" s="27"/>
+      <c r="I5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="28"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="9">
         <v>2</v>
       </c>
-      <c r="F5" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="45">
-        <v>7</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="46"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
-        <v>2</v>
-      </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1254,50 +1397,53 @@
         <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="15">
+        <v>42</v>
+      </c>
+      <c r="G6" s="8">
         <v>7.82</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="47"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="45" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="11">
-        <v>40.67</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="47"/>
-      <c r="K7" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-    </row>
-    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16">
+        <v>98</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="51">
+        <f>1590*2</f>
+        <v>3180</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="29"/>
+      <c r="L7" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="42"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1305,50 +1451,54 @@
         <v>1</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="11">
+        <v>42</v>
+      </c>
+      <c r="G8" s="7">
         <v>9.2799999999999994</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I8" s="47"/>
-    </row>
-    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16">
+      <c r="H8" s="51"/>
+      <c r="I8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="29"/>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9">
         <v>5</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="45"/>
+      <c r="D9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="9">
-        <v>2</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="47"/>
-      <c r="K9" s="22" t="s">
+      <c r="E9" s="23">
+        <v>4</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="49"/>
+      <c r="H9" s="52">
+        <v>120</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="48"/>
+      <c r="L9" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N9" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" s="24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="16">
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
         <v>6</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1356,30 +1506,31 @@
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="11">
+        <v>42</v>
+      </c>
+      <c r="G10" s="7">
         <v>3.5</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="51"/>
+      <c r="I10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="29"/>
+      <c r="L10" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="I10" s="47"/>
-      <c r="K10" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" s="31">
+      <c r="N10" s="69">
         <v>44809.72</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="16">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
         <v>7</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="45" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1389,30 +1540,31 @@
         <v>1</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="11">
+        <v>42</v>
+      </c>
+      <c r="G11" s="7">
         <v>7.33</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="51"/>
+      <c r="I11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="47"/>
-      <c r="K11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" s="17">
+      <c r="J11" s="29"/>
+      <c r="L11" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="72">
         <v>7987.01</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="16">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
         <v>8</v>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1420,24 +1572,31 @@
         <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="11">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7">
         <v>5.1100000000000003</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="51"/>
+      <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="47"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="17"/>
-    </row>
-    <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="16">
+      <c r="J12" s="29"/>
+      <c r="L12" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="M12" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" s="72">
+        <v>10041.09</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
         <v>9</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1445,503 +1604,662 @@
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="7">
+        <v>11.25</v>
+      </c>
+      <c r="H13" s="51"/>
+      <c r="I13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="29"/>
+      <c r="L13" s="70" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" s="72">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
+        <v>10</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="24">
+        <v>16.3</v>
+      </c>
+      <c r="H14" s="53"/>
+      <c r="I14" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="29"/>
+      <c r="L14" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="M14" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" s="72">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="9"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="59">
+        <v>2</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="61"/>
+      <c r="H15" s="62">
+        <v>200</v>
+      </c>
+      <c r="I15" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" s="29"/>
+      <c r="L15" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="M15" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="N15" s="72">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>11</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="23">
+        <v>1</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="24">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H16" s="53"/>
+      <c r="I16" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="29"/>
+      <c r="L16" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="M16" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="N16" s="66"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>12</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="D17" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="G13" s="11">
-        <v>11.25</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="47"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="62"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
-        <v>10</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="38">
-        <v>2</v>
-      </c>
-      <c r="F14" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="39">
-        <v>16.3</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="I14" s="47"/>
-      <c r="M14" s="63">
-        <f>SUM(M10:M13)</f>
-        <v>52796.73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="16">
-        <v>11</v>
-      </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="38">
-        <v>1</v>
-      </c>
-      <c r="F15" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="39">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="H15" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="47"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="16">
-        <v>12</v>
-      </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="11">
-        <v>3.92</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="47"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="16">
-        <v>13</v>
-      </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="11">
+        <v>42</v>
+      </c>
+      <c r="G17" s="7">
+        <v>3.92</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="29"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="10"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="9">
+        <v>13</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="7">
         <v>11.82</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H18" s="51"/>
+      <c r="I18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="29"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="10"/>
+    </row>
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9">
+        <v>14</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="47"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="16">
-        <v>14</v>
-      </c>
-      <c r="C18" s="42" t="s">
+      <c r="E19" s="23">
+        <v>5</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="53">
+        <v>150</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="J19" s="57"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="76"/>
+    </row>
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="9">
+        <v>15</v>
+      </c>
+      <c r="C20" s="45"/>
+      <c r="D20" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="23">
+        <v>2</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="53">
+        <v>60</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="57"/>
+      <c r="L20" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="M20" s="75"/>
+      <c r="N20" s="77">
+        <f>SUM(N10:N16)</f>
+        <v>68184.820000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="9">
+        <v>16</v>
+      </c>
+      <c r="C21" s="45"/>
+      <c r="D21" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="23">
+        <v>1</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="24">
+        <v>6.3</v>
+      </c>
+      <c r="H21" s="53"/>
+      <c r="I21" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="9">
+        <v>17</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="33">
+        <v>5</v>
+      </c>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="9">
+        <v>18</v>
+      </c>
+      <c r="C23" s="45"/>
+      <c r="D23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="7">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="H23" s="51"/>
+      <c r="I23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="29"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="9">
+        <v>19</v>
+      </c>
+      <c r="C24" s="45"/>
+      <c r="D24" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="23">
+        <v>5</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="49"/>
+      <c r="H24" s="52">
+        <v>100</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="57"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="9">
+        <v>20</v>
+      </c>
+      <c r="C25" s="45"/>
+      <c r="D25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="7">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="H25" s="51"/>
+      <c r="I25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="29"/>
+      <c r="M25" s="50"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="9">
+        <v>21</v>
+      </c>
+      <c r="C26" s="45"/>
+      <c r="D26" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="23">
+        <v>8</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="49"/>
+      <c r="H26" s="52">
+        <v>80</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="57"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="9">
+        <v>22</v>
+      </c>
+      <c r="C27" s="45"/>
+      <c r="D27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="7">
+        <v>4.21</v>
+      </c>
+      <c r="H27" s="51"/>
+      <c r="I27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="9">
+        <v>23</v>
+      </c>
+      <c r="C28" s="45"/>
+      <c r="D28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0.49</v>
+      </c>
+      <c r="H28" s="51"/>
+      <c r="I28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="29"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="9">
+        <v>24</v>
+      </c>
+      <c r="C29" s="45"/>
+      <c r="D29" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="23">
+        <v>3</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="24"/>
+      <c r="H29" s="53">
+        <v>939</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="9">
+        <v>25</v>
+      </c>
+      <c r="C30" s="45"/>
+      <c r="D30" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="23">
+        <v>2</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="63"/>
+      <c r="H30" s="53">
+        <v>120</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="9">
+        <v>26</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="23">
+        <v>11</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="24"/>
+      <c r="H31" s="53">
+        <v>550</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="57"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="9">
+        <v>27</v>
+      </c>
+      <c r="C32" s="45"/>
+      <c r="D32" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="18">
+        <v>2</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="54">
+        <v>10</v>
+      </c>
+      <c r="I32" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="9">
-        <v>5</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="47"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="16">
-        <v>15</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="5">
+      <c r="J32" s="29"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="9">
+        <v>28</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" s="29"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="9">
+        <v>29</v>
+      </c>
+      <c r="C34" s="42"/>
+      <c r="D34" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="J34" s="29"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="9">
+        <v>30</v>
+      </c>
+      <c r="C35" s="42"/>
+      <c r="D35" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="J35" s="29"/>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="30">
+        <v>31</v>
+      </c>
+      <c r="C36" s="43"/>
+      <c r="D36" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="31"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="73"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="73"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="73"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="73"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="73"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="13">
-        <v>0</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I19" s="47"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="16">
-        <v>16</v>
-      </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="38">
-        <v>1</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="39">
-        <v>6.3</v>
-      </c>
-      <c r="H20" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" s="47"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="16">
-        <v>17</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="53">
-        <v>5</v>
-      </c>
-      <c r="F21" s="53"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="47"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="16">
-        <v>18</v>
-      </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="11">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I22" s="47"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="16">
-        <v>19</v>
-      </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="9">
-        <v>5</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I23" s="47"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="16">
-        <v>20</v>
-      </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="11">
-        <v>17.489999999999998</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I24" s="47"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
-        <v>21</v>
-      </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="9">
-        <v>6</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="47"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="16">
-        <v>22</v>
-      </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="11">
-        <v>4.21</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I26" s="47"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="16">
-        <v>23</v>
-      </c>
-      <c r="C27" s="42"/>
-      <c r="D27" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" s="11">
-        <v>0.49</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="47"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="16">
-        <v>24</v>
-      </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="26">
-        <v>3</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" s="47"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="16">
-        <v>25</v>
-      </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="E29" s="26">
-        <v>2</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" s="32"/>
-      <c r="H29" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="I29" s="47"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="16">
-        <v>26</v>
-      </c>
-      <c r="C30" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="26">
-        <v>10</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="I30" s="47"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="16">
-        <v>27</v>
-      </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="26">
-        <v>2</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="I31" s="47"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="16">
+      <c r="F44" s="1"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="I32" s="47"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="16">
-        <v>29</v>
-      </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="I33" s="47"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="16">
-        <v>30</v>
-      </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="I34" s="47"/>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="48">
-        <v>31</v>
-      </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="57" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="57"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="51"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C43" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="1">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C29"/>
+  <mergeCells count="11">
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C30"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C14:C18"/>
     <mergeCell ref="C11:C13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{009E80E0-CC73-4407-97F9-5CA562932134}"/>
     <hyperlink ref="F9" r:id="rId2" xr:uid="{970E6C7B-CD83-4118-ACDC-8EB4789F8D02}"/>
-    <hyperlink ref="F25" r:id="rId3" xr:uid="{6848A319-9C3D-405C-8BEE-F33B21F3BF8F}"/>
-    <hyperlink ref="F23" r:id="rId4" xr:uid="{C8CE9F5A-42CF-4D2E-9D66-663D3AC2D43C}"/>
+    <hyperlink ref="F26" r:id="rId3" xr:uid="{6848A319-9C3D-405C-8BEE-F33B21F3BF8F}"/>
+    <hyperlink ref="F24" r:id="rId4" xr:uid="{C8CE9F5A-42CF-4D2E-9D66-663D3AC2D43C}"/>
     <hyperlink ref="F5" r:id="rId5" xr:uid="{216948AD-1941-48AF-8E3C-4F339182C1F8}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{19B7746E-DA4E-4FF7-AFFF-416CF5121261}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{2C572AA3-3AB0-425C-9B72-FA7FED21AC98}"/>
@@ -1949,25 +2267,27 @@
     <hyperlink ref="F11" r:id="rId9" xr:uid="{DA637D50-F2C3-47AD-A7C3-F7282BE9718E}"/>
     <hyperlink ref="F12" r:id="rId10" xr:uid="{6BCB2BB9-5F6C-4371-8A4D-683495B420E2}"/>
     <hyperlink ref="F13" r:id="rId11" xr:uid="{5EBB2BDD-A40B-44FD-B413-BBABC10CA771}"/>
-    <hyperlink ref="F16" r:id="rId12" xr:uid="{3115B913-2711-4AC4-A3F3-96AC7B7D7417}"/>
-    <hyperlink ref="F17" r:id="rId13" xr:uid="{6D96920C-4613-4E82-8AB7-196EDDCA5789}"/>
-    <hyperlink ref="F22" r:id="rId14" xr:uid="{FFD2E4E6-8F53-4D02-BD72-F2353835E98E}"/>
-    <hyperlink ref="F24" r:id="rId15" xr:uid="{D53C4188-224B-4190-91FC-BDD4B0CE1088}"/>
-    <hyperlink ref="F26" r:id="rId16" xr:uid="{2BDB80E1-F69C-4A65-BE00-E96747144E0E}"/>
-    <hyperlink ref="F27" r:id="rId17" xr:uid="{A1216382-173D-4DE8-8B55-B8AA0B432E5E}"/>
-    <hyperlink ref="F30" r:id="rId18" xr:uid="{537B03B5-DE99-4376-A395-EA76E9416915}"/>
-    <hyperlink ref="F31" r:id="rId19" xr:uid="{A76581A8-80D9-4C32-A637-E5C30AC9CBF4}"/>
-    <hyperlink ref="F29" r:id="rId20" xr:uid="{F420E434-709D-4376-89CE-505F92CFCB33}"/>
-    <hyperlink ref="F28" r:id="rId21" xr:uid="{D9718443-4813-40E0-A6BD-4DB2D05599CE}"/>
-    <hyperlink ref="F20" r:id="rId22" xr:uid="{F59BDD79-BCAE-4D71-A0F6-00F6DD647236}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{3115B913-2711-4AC4-A3F3-96AC7B7D7417}"/>
+    <hyperlink ref="F18" r:id="rId13" xr:uid="{6D96920C-4613-4E82-8AB7-196EDDCA5789}"/>
+    <hyperlink ref="F23" r:id="rId14" xr:uid="{FFD2E4E6-8F53-4D02-BD72-F2353835E98E}"/>
+    <hyperlink ref="F25" r:id="rId15" xr:uid="{D53C4188-224B-4190-91FC-BDD4B0CE1088}"/>
+    <hyperlink ref="F27" r:id="rId16" xr:uid="{2BDB80E1-F69C-4A65-BE00-E96747144E0E}"/>
+    <hyperlink ref="F28" r:id="rId17" xr:uid="{A1216382-173D-4DE8-8B55-B8AA0B432E5E}"/>
+    <hyperlink ref="F31" r:id="rId18" xr:uid="{537B03B5-DE99-4376-A395-EA76E9416915}"/>
+    <hyperlink ref="F32" r:id="rId19" xr:uid="{A76581A8-80D9-4C32-A637-E5C30AC9CBF4}"/>
+    <hyperlink ref="F30" r:id="rId20" xr:uid="{F420E434-709D-4376-89CE-505F92CFCB33}"/>
+    <hyperlink ref="F29" r:id="rId21" xr:uid="{D9718443-4813-40E0-A6BD-4DB2D05599CE}"/>
+    <hyperlink ref="F21" r:id="rId22" xr:uid="{F59BDD79-BCAE-4D71-A0F6-00F6DD647236}"/>
     <hyperlink ref="F14" r:id="rId23" xr:uid="{19004DEF-B628-42C8-A319-B93D75C99EBE}"/>
-    <hyperlink ref="F15" r:id="rId24" xr:uid="{DDA70933-F519-4120-A62F-796F89685867}"/>
-    <hyperlink ref="F19" r:id="rId25" xr:uid="{2DC38031-1606-4CF1-A8A4-2C5BD8230223}"/>
-    <hyperlink ref="H32" r:id="rId26" xr:uid="{729AFFBF-612D-4688-AA55-A58EEB43BE1F}"/>
-    <hyperlink ref="H33" r:id="rId27" xr:uid="{E57884CF-A747-4A22-8C0C-AB80E3119C1B}"/>
-    <hyperlink ref="H34" r:id="rId28" xr:uid="{D4740D64-7161-44CD-A885-4A3132632838}"/>
+    <hyperlink ref="F16" r:id="rId24" xr:uid="{DDA70933-F519-4120-A62F-796F89685867}"/>
+    <hyperlink ref="F20" r:id="rId25" xr:uid="{2DC38031-1606-4CF1-A8A4-2C5BD8230223}"/>
+    <hyperlink ref="I33" r:id="rId26" xr:uid="{729AFFBF-612D-4688-AA55-A58EEB43BE1F}"/>
+    <hyperlink ref="I34" r:id="rId27" xr:uid="{E57884CF-A747-4A22-8C0C-AB80E3119C1B}"/>
+    <hyperlink ref="I35" r:id="rId28" xr:uid="{D4740D64-7161-44CD-A885-4A3132632838}"/>
+    <hyperlink ref="F19" r:id="rId29" xr:uid="{119FC45D-9FAB-4BF2-8E22-B59C5FAA658F}"/>
+    <hyperlink ref="F15" r:id="rId30" xr:uid="{499CDB06-8D3F-463D-8761-4931B93C72DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="62" orientation="landscape" r:id="rId29"/>
+  <pageSetup scale="62" orientation="landscape" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Readme File V0.1: Until PCB design
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofmora-my.sharepoint.com/personal/fernandopbm_19_uom_lk/Documents/Volume D/Competitions/micromouse/NewGIT/SINDiB-MicroMouse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\SINDiB-MICROMOUSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D8307B-E79E-44A3-B8A0-95169180C92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B02E64D-54F5-43BC-A5A3-BBBD04FCC7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="102">
   <si>
     <t>COMPONENT</t>
   </si>
@@ -290,12 +290,6 @@
     <t>3.7V,  (Aliexpress - 5 - 800mAh with charger)</t>
   </si>
   <si>
-    <t>Low Drop Voltage - 5V Linear Regulator</t>
-  </si>
-  <si>
-    <t>Low Drop Voltage - 3.3V Linear Regulator</t>
-  </si>
-  <si>
     <t>3-SPDTT Slide Switch</t>
   </si>
   <si>
@@ -332,9 +326,6 @@
     <t>16MHz, 2Pin SMD</t>
   </si>
   <si>
-    <t>Chamith</t>
-  </si>
-  <si>
     <t>Duino</t>
   </si>
   <si>
@@ -342,6 +333,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Biyon</t>
+  </si>
+  <si>
+    <t>Custom-Clearance</t>
+  </si>
+  <si>
+    <t>Low Drop Voltage - 5V Linear Regulator (MIC39101)</t>
+  </si>
+  <si>
+    <t>Low Drop Voltage - 3.3V Linear Regulator (TLV76733)</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,12 +468,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -815,7 +812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -862,7 +859,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -888,7 +884,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -910,7 +905,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -923,17 +918,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -958,6 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1286,47 +1282,47 @@
   <dimension ref="B1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
-    <col min="7" max="8" width="16.44140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="66.44140625" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="66.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="72" t="s">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="L2" s="40" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="L2" s="39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L3" s="41" t="s">
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1343,10 +1339,10 @@
         <v>41</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>4</v>
@@ -1354,15 +1350,15 @@
       <c r="J4" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="39" t="s">
+      <c r="L4" s="38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="11" t="s">
@@ -1381,13 +1377,13 @@
       <c r="I5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J5" s="74"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>2</v>
       </c>
-      <c r="C6" s="73"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1404,13 +1400,13 @@
       <c r="I6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="29"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J6" s="48"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="71" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1420,28 +1416,28 @@
         <v>2</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="44">
+      <c r="H7" s="42">
         <f>1590*2</f>
         <v>3180</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="L7" s="74" t="s">
+      <c r="J7" s="48"/>
+      <c r="L7" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-    </row>
-    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="73"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1454,17 +1450,17 @@
       <c r="G8" s="7">
         <v>9.2799999999999994</v>
       </c>
-      <c r="H8" s="44"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J8" s="29"/>
-    </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="J8" s="48"/>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>5</v>
       </c>
-      <c r="C9" s="73"/>
+      <c r="C9" s="71"/>
       <c r="D9" s="22" t="s">
         <v>10</v>
       </c>
@@ -1474,14 +1470,14 @@
       <c r="F9" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="45">
+      <c r="G9" s="41"/>
+      <c r="H9" s="43">
         <v>120</v>
       </c>
       <c r="I9" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="42"/>
+      <c r="J9" s="48"/>
       <c r="L9" s="15" t="s">
         <v>51</v>
       </c>
@@ -1492,11 +1488,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>6</v>
       </c>
-      <c r="C10" s="73"/>
+      <c r="C10" s="71"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1509,26 +1505,26 @@
       <c r="G10" s="7">
         <v>3.5</v>
       </c>
-      <c r="H10" s="44"/>
+      <c r="H10" s="42"/>
       <c r="I10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" s="29"/>
-      <c r="L10" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="J10" s="48"/>
+      <c r="L10" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="M10" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="N10" s="62">
+      <c r="M10" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="N10" s="60">
         <v>44809.72</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
         <v>7</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="71" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1543,26 +1539,26 @@
       <c r="G11" s="7">
         <v>7.33</v>
       </c>
-      <c r="H11" s="44"/>
+      <c r="H11" s="42"/>
       <c r="I11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="L11" s="63" t="s">
+      <c r="J11" s="28"/>
+      <c r="L11" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="M11" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="N11" s="65">
+      <c r="M11" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="N11" s="63">
         <v>7987.01</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
         <v>8</v>
       </c>
-      <c r="C12" s="73"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1575,26 +1571,26 @@
       <c r="G12" s="7">
         <v>5.1100000000000003</v>
       </c>
-      <c r="H12" s="44"/>
+      <c r="H12" s="42"/>
       <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="29"/>
-      <c r="L12" s="63" t="s">
+      <c r="J12" s="28"/>
+      <c r="L12" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="M12" s="64" t="s">
-        <v>99</v>
-      </c>
-      <c r="N12" s="65">
+      <c r="M12" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="63">
         <v>10041.09</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>9</v>
       </c>
-      <c r="C13" s="73"/>
+      <c r="C13" s="71"/>
       <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1607,26 +1603,26 @@
       <c r="G13" s="7">
         <v>11.25</v>
       </c>
-      <c r="H13" s="44"/>
+      <c r="H13" s="42"/>
       <c r="I13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="29"/>
-      <c r="L13" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="M13" s="64" t="s">
+      <c r="J13" s="48"/>
+      <c r="L13" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="M13" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="N13" s="65">
+      <c r="N13" s="63">
         <v>1228</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
         <v>10</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="71" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="22" t="s">
@@ -1641,56 +1637,56 @@
       <c r="G14" s="24">
         <v>16.3</v>
       </c>
-      <c r="H14" s="46"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="L14" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="M14" s="64" t="s">
+      <c r="J14" s="28"/>
+      <c r="L14" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="N14" s="65">
-        <v>3180</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M14" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="N14" s="63">
+        <v>4671.6899999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="51" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="52">
+      <c r="C15" s="71"/>
+      <c r="D15" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="50">
         <v>2</v>
       </c>
-      <c r="F15" s="53" t="s">
+      <c r="F15" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="54"/>
-      <c r="H15" s="55">
+      <c r="G15" s="52"/>
+      <c r="H15" s="53">
         <v>200</v>
       </c>
-      <c r="I15" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="J15" s="29"/>
-      <c r="L15" s="63" t="s">
+      <c r="I15" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="28"/>
+      <c r="L15" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="N15" s="65">
+      <c r="M15" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" s="63">
         <v>939</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>11</v>
       </c>
-      <c r="C16" s="73"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="23" t="s">
         <v>72</v>
       </c>
@@ -1703,24 +1699,24 @@
       <c r="G16" s="24">
         <v>1.1399999999999999</v>
       </c>
-      <c r="H16" s="46"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="L16" s="57" t="s">
+      <c r="J16" s="28"/>
+      <c r="L16" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="N16" s="59"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="M16" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="N16" s="57"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>12</v>
       </c>
-      <c r="C17" s="73"/>
+      <c r="C17" s="71"/>
       <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1733,20 +1729,26 @@
       <c r="G17" s="7">
         <v>3.92</v>
       </c>
-      <c r="H17" s="44"/>
+      <c r="H17" s="42"/>
       <c r="I17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J17" s="29"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="10"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J17" s="48"/>
+      <c r="L17" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="M17" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="N17" s="63">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>13</v>
       </c>
-      <c r="C18" s="73"/>
+      <c r="C18" s="71"/>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1759,20 +1761,20 @@
       <c r="G18" s="7">
         <v>11.82</v>
       </c>
-      <c r="H18" s="44"/>
+      <c r="H18" s="42"/>
       <c r="I18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J18" s="29"/>
+      <c r="J18" s="48"/>
       <c r="L18" s="9"/>
       <c r="M18" s="2"/>
       <c r="N18" s="10"/>
     </row>
-    <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
         <v>14</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="71" t="s">
         <v>60</v>
       </c>
       <c r="D19" s="23" t="s">
@@ -1785,22 +1787,22 @@
         <v>56</v>
       </c>
       <c r="G19" s="24"/>
-      <c r="H19" s="46">
+      <c r="H19" s="44">
         <v>150</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="J19" s="50"/>
+        <v>84</v>
+      </c>
+      <c r="J19" s="48"/>
       <c r="L19" s="9"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="66"/>
-    </row>
-    <row r="20" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N19" s="64"/>
+    </row>
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
         <v>15</v>
       </c>
-      <c r="C20" s="73"/>
+      <c r="C20" s="71"/>
       <c r="D20" s="23" t="s">
         <v>62</v>
       </c>
@@ -1811,27 +1813,27 @@
         <v>56</v>
       </c>
       <c r="G20" s="24"/>
-      <c r="H20" s="46">
+      <c r="H20" s="44">
         <v>60</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J20" s="50"/>
-      <c r="L20" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="M20" s="69"/>
-      <c r="N20" s="67">
-        <f>SUM(N10:N16)</f>
-        <v>68184.820000000007</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="J20" s="48"/>
+      <c r="L20" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="M20" s="67"/>
+      <c r="N20" s="65">
+        <f>SUM(N10:N17)</f>
+        <v>71814.510000000009</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="9">
         <v>16</v>
       </c>
-      <c r="C21" s="73"/>
+      <c r="C21" s="71"/>
       <c r="D21" s="23" t="s">
         <v>61</v>
       </c>
@@ -1844,38 +1846,38 @@
       <c r="G21" s="24">
         <v>6.3</v>
       </c>
-      <c r="H21" s="46"/>
+      <c r="H21" s="44"/>
       <c r="I21" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="J21" s="29"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J21" s="28"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>17</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="32">
         <v>5</v>
       </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="33" t="s">
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="29"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J22" s="28"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="9">
         <v>18</v>
       </c>
-      <c r="C23" s="73"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="2" t="s">
         <v>35</v>
       </c>
@@ -1888,17 +1890,17 @@
       <c r="G23" s="7">
         <v>4.1100000000000003</v>
       </c>
-      <c r="H23" s="44"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J23" s="29"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J23" s="48"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
         <v>19</v>
       </c>
-      <c r="C24" s="73"/>
+      <c r="C24" s="71"/>
       <c r="D24" s="23" t="s">
         <v>30</v>
       </c>
@@ -1908,20 +1910,20 @@
       <c r="F24" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="43"/>
-      <c r="H24" s="45">
+      <c r="G24" s="41"/>
+      <c r="H24" s="43">
         <v>100</v>
       </c>
       <c r="I24" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J24" s="50"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J24" s="48"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>20</v>
       </c>
-      <c r="C25" s="73"/>
+      <c r="C25" s="71"/>
       <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1934,17 +1936,17 @@
       <c r="G25" s="7">
         <v>17.489999999999998</v>
       </c>
-      <c r="H25" s="44"/>
+      <c r="H25" s="42"/>
       <c r="I25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J25" s="29"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J25" s="48"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="9">
         <v>21</v>
       </c>
-      <c r="C26" s="73"/>
+      <c r="C26" s="71"/>
       <c r="D26" s="23" t="s">
         <v>34</v>
       </c>
@@ -1954,20 +1956,20 @@
       <c r="F26" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="43"/>
-      <c r="H26" s="45">
+      <c r="G26" s="41"/>
+      <c r="H26" s="43">
         <v>80</v>
       </c>
       <c r="I26" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J26" s="50"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J26" s="48"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="9">
         <v>22</v>
       </c>
-      <c r="C27" s="73"/>
+      <c r="C27" s="71"/>
       <c r="D27" s="2" t="s">
         <v>47</v>
       </c>
@@ -1980,17 +1982,17 @@
       <c r="G27" s="7">
         <v>4.21</v>
       </c>
-      <c r="H27" s="44"/>
+      <c r="H27" s="42"/>
       <c r="I27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J27" s="29"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J27" s="48"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
         <v>23</v>
       </c>
-      <c r="C28" s="73"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="2" t="s">
         <v>31</v>
       </c>
@@ -2003,17 +2005,17 @@
       <c r="G28" s="7">
         <v>0.49</v>
       </c>
-      <c r="H28" s="44"/>
+      <c r="H28" s="42"/>
       <c r="I28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="29"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J28" s="48"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="9">
         <v>24</v>
       </c>
-      <c r="C29" s="73"/>
+      <c r="C29" s="71"/>
       <c r="D29" s="23" t="s">
         <v>68</v>
       </c>
@@ -2021,22 +2023,22 @@
         <v>3</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G29" s="24"/>
-      <c r="H29" s="46">
+      <c r="H29" s="44">
         <v>939</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="J29" s="29"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="J29" s="28"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="9">
         <v>25</v>
       </c>
-      <c r="C30" s="73"/>
+      <c r="C30" s="71"/>
       <c r="D30" s="23" t="s">
         <v>58</v>
       </c>
@@ -2046,20 +2048,20 @@
       <c r="F30" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="56"/>
-      <c r="H30" s="46">
+      <c r="G30" s="54"/>
+      <c r="H30" s="44">
         <v>120</v>
       </c>
       <c r="I30" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="J30" s="29"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J30" s="48"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="9">
         <v>26</v>
       </c>
-      <c r="C31" s="73" t="s">
+      <c r="C31" s="71" t="s">
         <v>57</v>
       </c>
       <c r="D31" s="22" t="s">
@@ -2072,19 +2074,19 @@
         <v>56</v>
       </c>
       <c r="G31" s="24"/>
-      <c r="H31" s="46">
+      <c r="H31" s="44">
         <v>550</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="50"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J31" s="48"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="9">
         <v>27</v>
       </c>
-      <c r="C32" s="73"/>
+      <c r="C32" s="71"/>
       <c r="D32" s="18" t="s">
         <v>59</v>
       </c>
@@ -2095,103 +2097,103 @@
         <v>56</v>
       </c>
       <c r="G32" s="20"/>
-      <c r="H32" s="47">
+      <c r="H32" s="45">
         <v>10</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="29"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J32" s="28"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="9">
         <v>28</v>
       </c>
-      <c r="C33" s="70" t="s">
+      <c r="C33" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="35" t="s">
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J33" s="29"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J33" s="28"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="9">
         <v>29</v>
       </c>
-      <c r="C34" s="70"/>
-      <c r="D34" s="33" t="s">
+      <c r="C34" s="68"/>
+      <c r="D34" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="35" t="s">
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J34" s="29"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J34" s="28"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="9">
         <v>30</v>
       </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="33" t="s">
+      <c r="C35" s="68"/>
+      <c r="D35" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="35" t="s">
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J35" s="29"/>
-    </row>
-    <row r="36" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="30">
+      <c r="J35" s="28"/>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="29">
         <v>31</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="37" t="s">
+      <c r="C36" s="69"/>
+      <c r="D36" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="31"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="30"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G38"/>
       <c r="H38"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G39"/>
       <c r="H39"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G40"/>
       <c r="H40"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G41"/>
       <c r="H41"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G42"/>
       <c r="H42"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
V0.2: Availablity Update to Components
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\SINDiB-MicroMouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\SINDiB-MICROMOUSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96DC3CE-0C33-490E-BFF2-C1FCD3A526D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A0CE99-59C6-4EEE-B213-E4DF6E902579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
   <si>
     <t>COMPONENT</t>
   </si>
@@ -460,6 +471,9 @@
   </si>
   <si>
     <t>AVAILABLE</t>
+  </si>
+  <si>
+    <t>Expected Order</t>
   </si>
 </sst>
 </file>
@@ -520,7 +534,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,6 +625,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="30">
     <border>
@@ -1012,7 +1032,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1057,10 +1077,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1083,9 +1099,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1110,106 +1123,114 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1537,48 +1558,48 @@
   </sheetPr>
   <dimension ref="B1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
-    <col min="7" max="8" width="16.44140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="66.44140625" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" customWidth="1"/>
-    <col min="13" max="13" width="24.44140625" customWidth="1"/>
-    <col min="14" max="14" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="66.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="62" t="s">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="L2" s="31" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="L2" s="29" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L3" s="32" t="s">
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
@@ -1606,15 +1627,15 @@
       <c r="J4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="81" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1633,13 +1654,13 @@
       <c r="I5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="57"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J5" s="53"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="63"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1656,13 +1677,13 @@
       <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="39"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J6" s="36"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="79" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1675,25 +1696,25 @@
         <v>92</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="34">
+      <c r="H7" s="32">
         <f>1590*2</f>
         <v>3180</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="39"/>
-      <c r="L7" s="64" t="s">
+      <c r="J7" s="36"/>
+      <c r="L7" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-    </row>
-    <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="63"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1706,17 +1727,17 @@
       <c r="G8" s="5">
         <v>9.2799999999999994</v>
       </c>
-      <c r="H8" s="34"/>
+      <c r="H8" s="32"/>
       <c r="I8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J8" s="36"/>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="20" t="s">
         <v>10</v>
       </c>
@@ -1726,14 +1747,14 @@
       <c r="F9" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="35">
+      <c r="G9" s="31"/>
+      <c r="H9" s="33">
         <v>120</v>
       </c>
       <c r="I9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="39"/>
+      <c r="J9" s="36"/>
       <c r="L9" s="13" t="s">
         <v>49</v>
       </c>
@@ -1744,11 +1765,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="63"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1761,26 +1782,26 @@
       <c r="G10" s="5">
         <v>3.5</v>
       </c>
-      <c r="H10" s="34"/>
+      <c r="H10" s="32"/>
       <c r="I10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="39"/>
-      <c r="L10" s="49" t="s">
+      <c r="J10" s="36"/>
+      <c r="L10" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="M10" s="50" t="s">
+      <c r="M10" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="N10" s="51">
+      <c r="N10" s="48">
         <v>44809.72</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="79" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1795,26 +1816,26 @@
       <c r="G11" s="5">
         <v>7.33</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="32"/>
       <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J11" s="26"/>
-      <c r="L11" s="52" t="s">
+      <c r="L11" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="53" t="s">
+      <c r="M11" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="N11" s="54">
+      <c r="N11" s="51">
         <v>7987.01</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="63"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1827,26 +1848,26 @@
       <c r="G12" s="5">
         <v>5.1100000000000003</v>
       </c>
-      <c r="H12" s="34"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="26"/>
-      <c r="L12" s="52" t="s">
+      <c r="L12" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="53" t="s">
+      <c r="M12" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="N12" s="54">
+      <c r="N12" s="51">
         <v>10041.09</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>9</v>
       </c>
-      <c r="C13" s="63"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1859,26 +1880,26 @@
       <c r="G13" s="5">
         <v>11.25</v>
       </c>
-      <c r="H13" s="34"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="39"/>
-      <c r="L13" s="52" t="s">
+      <c r="J13" s="36"/>
+      <c r="L13" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="M13" s="53" t="s">
+      <c r="M13" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="54">
+      <c r="N13" s="51">
         <v>1228</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>10</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="79" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -1893,56 +1914,56 @@
       <c r="G14" s="22">
         <v>16.3</v>
       </c>
-      <c r="H14" s="36"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="21" t="s">
         <v>69</v>
       </c>
       <c r="J14" s="26"/>
-      <c r="L14" s="52" t="s">
+      <c r="L14" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="M14" s="53" t="s">
+      <c r="M14" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="N14" s="54">
+      <c r="N14" s="51">
         <v>4671.6899999999996</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="40" t="s">
+      <c r="C15" s="79"/>
+      <c r="D15" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="38">
         <v>2</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44">
+      <c r="G15" s="40"/>
+      <c r="H15" s="41">
         <v>200</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="38" t="s">
         <v>90</v>
       </c>
       <c r="J15" s="26"/>
-      <c r="L15" s="52" t="s">
+      <c r="L15" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="M15" s="53" t="s">
+      <c r="M15" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="54">
+      <c r="N15" s="51">
         <v>939</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>11</v>
       </c>
-      <c r="C16" s="63"/>
+      <c r="C16" s="79"/>
       <c r="D16" s="21" t="s">
         <v>70</v>
       </c>
@@ -1955,26 +1976,26 @@
       <c r="G16" s="22">
         <v>1.1399999999999999</v>
       </c>
-      <c r="H16" s="36"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="39"/>
-      <c r="L16" s="46" t="s">
+      <c r="J16" s="36"/>
+      <c r="L16" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="M16" s="47" t="s">
+      <c r="M16" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="N16" s="48">
+      <c r="N16" s="45">
         <v>-13709.74</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>12</v>
       </c>
-      <c r="C17" s="63"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1987,26 +2008,26 @@
       <c r="G17" s="5">
         <v>3.92</v>
       </c>
-      <c r="H17" s="34"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="39"/>
-      <c r="L17" s="52" t="s">
+      <c r="J17" s="36"/>
+      <c r="L17" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="M17" s="53" t="s">
+      <c r="M17" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="N17" s="54">
+      <c r="N17" s="51">
         <v>2138</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>13</v>
       </c>
-      <c r="C18" s="63"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2019,26 +2040,27 @@
       <c r="G18" s="5">
         <v>11.82</v>
       </c>
-      <c r="H18" s="34"/>
+      <c r="H18" s="32"/>
       <c r="I18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="39"/>
-      <c r="L18" s="52" t="s">
+      <c r="J18" s="36"/>
+      <c r="L18" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="M18" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="N18" s="54">
-        <v>1685</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M18" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="N18" s="51">
+        <f>1685+180</f>
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>14</v>
       </c>
-      <c r="C19" s="63" t="s">
+      <c r="C19" s="79" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="21" t="s">
@@ -2051,29 +2073,29 @@
         <v>54</v>
       </c>
       <c r="G19" s="22"/>
-      <c r="H19" s="36">
+      <c r="H19" s="34">
         <v>150</v>
       </c>
       <c r="I19" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="J19" s="39"/>
-      <c r="L19" s="52" t="s">
+      <c r="J19" s="36"/>
+      <c r="L19" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="M19" s="53" t="s">
+      <c r="M19" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="N19" s="75">
+      <c r="N19" s="60">
         <f>240+190</f>
         <v>430</v>
       </c>
     </row>
-    <row r="20" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>15</v>
       </c>
-      <c r="C20" s="63"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="21" t="s">
         <v>60</v>
       </c>
@@ -2084,27 +2106,27 @@
         <v>54</v>
       </c>
       <c r="G20" s="22"/>
-      <c r="H20" s="36">
+      <c r="H20" s="34">
         <v>60</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="39"/>
-      <c r="L20" s="58" t="s">
+      <c r="J20" s="36"/>
+      <c r="L20" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="M20" s="59"/>
-      <c r="N20" s="56">
+      <c r="M20" s="75"/>
+      <c r="N20" s="52">
         <f>SUM(N10:N19)</f>
-        <v>60219.770000000011</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+        <v>60399.770000000011</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>16</v>
       </c>
-      <c r="C21" s="63"/>
+      <c r="C21" s="79"/>
       <c r="D21" s="21" t="s">
         <v>59</v>
       </c>
@@ -2117,38 +2139,42 @@
       <c r="G21" s="22">
         <v>6.3</v>
       </c>
-      <c r="H21" s="36"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="21" t="s">
         <v>68</v>
       </c>
       <c r="J21" s="26"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <v>17</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="28">
-        <v>5</v>
-      </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="28" t="s">
+      <c r="E22" s="82">
+        <v>6</v>
+      </c>
+      <c r="F22" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="83"/>
+      <c r="H22" s="84">
+        <v>180</v>
+      </c>
+      <c r="I22" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="26"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J22" s="36"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <v>18</v>
       </c>
-      <c r="C23" s="63"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2161,17 +2187,17 @@
       <c r="G23" s="5">
         <v>4.1100000000000003</v>
       </c>
-      <c r="H23" s="34"/>
+      <c r="H23" s="32"/>
       <c r="I23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="39"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J23" s="36"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>19</v>
       </c>
-      <c r="C24" s="63"/>
+      <c r="C24" s="79"/>
       <c r="D24" s="21" t="s">
         <v>28</v>
       </c>
@@ -2181,20 +2207,20 @@
       <c r="F24" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="35">
+      <c r="G24" s="31"/>
+      <c r="H24" s="33">
         <v>100</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="39"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J24" s="36"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <v>20</v>
       </c>
-      <c r="C25" s="63"/>
+      <c r="C25" s="79"/>
       <c r="D25" s="1" t="s">
         <v>27</v>
       </c>
@@ -2207,17 +2233,17 @@
       <c r="G25" s="5">
         <v>17.489999999999998</v>
       </c>
-      <c r="H25" s="34"/>
+      <c r="H25" s="32"/>
       <c r="I25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J25" s="39"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J25" s="36"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <v>21</v>
       </c>
-      <c r="C26" s="63"/>
+      <c r="C26" s="79"/>
       <c r="D26" s="21" t="s">
         <v>32</v>
       </c>
@@ -2227,20 +2253,20 @@
       <c r="F26" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="35">
+      <c r="G26" s="31"/>
+      <c r="H26" s="33">
         <v>80</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J26" s="36"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <v>22</v>
       </c>
-      <c r="C27" s="63"/>
+      <c r="C27" s="79"/>
       <c r="D27" s="1" t="s">
         <v>45</v>
       </c>
@@ -2253,17 +2279,17 @@
       <c r="G27" s="5">
         <v>4.21</v>
       </c>
-      <c r="H27" s="34"/>
+      <c r="H27" s="32"/>
       <c r="I27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J27" s="36"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
         <v>23</v>
       </c>
-      <c r="C28" s="63"/>
+      <c r="C28" s="79"/>
       <c r="D28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2276,17 +2302,17 @@
       <c r="G28" s="5">
         <v>0.49</v>
       </c>
-      <c r="H28" s="34"/>
+      <c r="H28" s="32"/>
       <c r="I28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J28" s="39"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J28" s="36"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
         <v>24</v>
       </c>
-      <c r="C29" s="63"/>
+      <c r="C29" s="79"/>
       <c r="D29" s="21" t="s">
         <v>66</v>
       </c>
@@ -2297,19 +2323,19 @@
         <v>82</v>
       </c>
       <c r="G29" s="22"/>
-      <c r="H29" s="36">
+      <c r="H29" s="34">
         <v>939</v>
       </c>
       <c r="I29" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="J29" s="39"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J29" s="36"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
         <v>25</v>
       </c>
-      <c r="C30" s="63"/>
+      <c r="C30" s="79"/>
       <c r="D30" s="21" t="s">
         <v>56</v>
       </c>
@@ -2319,20 +2345,20 @@
       <c r="F30" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="45"/>
-      <c r="H30" s="36">
+      <c r="G30" s="42"/>
+      <c r="H30" s="34">
         <v>120</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="39"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J30" s="36"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="7">
         <v>26</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="79" t="s">
         <v>55</v>
       </c>
       <c r="D31" s="20" t="s">
@@ -2345,19 +2371,19 @@
         <v>54</v>
       </c>
       <c r="G31" s="22"/>
-      <c r="H31" s="36">
+      <c r="H31" s="34">
         <v>550</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="39"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="J31" s="36"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="7">
         <v>27</v>
       </c>
-      <c r="C32" s="63"/>
+      <c r="C32" s="79"/>
       <c r="D32" s="16" t="s">
         <v>57</v>
       </c>
@@ -2368,7 +2394,7 @@
         <v>54</v>
       </c>
       <c r="G32" s="18"/>
-      <c r="H32" s="37">
+      <c r="H32" s="35">
         <v>10</v>
       </c>
       <c r="I32" s="16" t="s">
@@ -2376,738 +2402,875 @@
       </c>
       <c r="J32" s="26"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="7">
         <v>28</v>
       </c>
-      <c r="C33" s="60" t="s">
+      <c r="C33" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="66" t="s">
+      <c r="D33" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="E33" s="67">
-        <v>1</v>
-      </c>
-      <c r="F33" s="67" t="s">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G33" s="68"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="70" t="s">
+      <c r="G33" s="5"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="J33" s="39"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J33" s="36"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="7">
         <v>29</v>
       </c>
-      <c r="C34" s="60"/>
-      <c r="D34" s="67" t="s">
+      <c r="C34" s="76"/>
+      <c r="D34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="67">
-        <v>1</v>
-      </c>
-      <c r="F34" s="70" t="s">
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="G34" s="71"/>
-      <c r="H34" s="69">
+      <c r="G34" s="56"/>
+      <c r="H34" s="32">
         <v>160</v>
       </c>
-      <c r="I34" s="70" t="s">
+      <c r="I34" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="J34" s="39"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J34" s="36"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="7">
         <v>30</v>
       </c>
-      <c r="C35" s="60"/>
-      <c r="D35" s="67" t="s">
+      <c r="C35" s="76"/>
+      <c r="D35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="67">
-        <v>1</v>
-      </c>
-      <c r="F35" s="70" t="s">
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="G35" s="71"/>
-      <c r="H35" s="69">
+      <c r="G35" s="56"/>
+      <c r="H35" s="32">
         <v>1375</v>
       </c>
-      <c r="I35" s="70" t="s">
+      <c r="I35" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J35" s="36"/>
+    </row>
+    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="27">
         <v>31</v>
       </c>
-      <c r="C36" s="61"/>
-      <c r="D36" s="72" t="s">
+      <c r="C36" s="77"/>
+      <c r="D36" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="72">
-        <v>1</v>
-      </c>
-      <c r="F36" s="72" t="s">
+      <c r="E36" s="57">
+        <v>1</v>
+      </c>
+      <c r="F36" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="G36" s="73"/>
-      <c r="H36" s="74">
+      <c r="G36" s="58"/>
+      <c r="H36" s="59">
         <v>175</v>
       </c>
-      <c r="I36" s="72" t="s">
+      <c r="I36" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="J36" s="76"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="79"/>
+      <c r="J36" s="61"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G38"/>
       <c r="H38"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C39" s="80" t="s">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
       <c r="G39"/>
       <c r="H39"/>
     </row>
-    <row r="40" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G40"/>
       <c r="H40"/>
     </row>
-    <row r="41" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="91"/>
-      <c r="C41" s="92" t="s">
+    <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="62"/>
+      <c r="C41" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="92" t="s">
+      <c r="D41" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="93" t="s">
+      <c r="E41" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="G41" s="108" t="s">
+      <c r="G41" s="100" t="s">
         <v>143</v>
       </c>
-      <c r="H41"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B42" s="94">
-        <v>1</v>
-      </c>
-      <c r="C42" s="95" t="s">
+      <c r="H41" s="101" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="65">
+        <v>1</v>
+      </c>
+      <c r="C42" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" s="96">
-        <v>1</v>
-      </c>
-      <c r="G42" s="104"/>
-      <c r="H42"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D42" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="87">
+        <v>1</v>
+      </c>
+      <c r="G42" s="65">
+        <v>1</v>
+      </c>
+      <c r="H42" s="110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="7">
         <v>2</v>
       </c>
-      <c r="C43" s="81" t="s">
+      <c r="C43" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="8">
-        <v>1</v>
-      </c>
-      <c r="G43" s="105"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E43" s="88">
+        <v>1</v>
+      </c>
+      <c r="G43" s="102">
+        <v>3</v>
+      </c>
+      <c r="H43" s="111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="7">
         <v>3</v>
       </c>
-      <c r="C44" s="83"/>
-      <c r="D44" s="67" t="s">
+      <c r="C44" s="69"/>
+      <c r="D44" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="97">
-        <v>1</v>
-      </c>
-      <c r="F44" s="77"/>
-      <c r="G44" s="106"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="77"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E44" s="106">
+        <v>1</v>
+      </c>
+      <c r="G44" s="102">
+        <v>3</v>
+      </c>
+      <c r="H44" s="111">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="7">
         <v>4</v>
       </c>
-      <c r="C45" s="82"/>
-      <c r="D45" s="67" t="s">
+      <c r="C45" s="70"/>
+      <c r="D45" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="97">
-        <v>1</v>
-      </c>
-      <c r="G45" s="105"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E45" s="88">
+        <v>1</v>
+      </c>
+      <c r="G45" s="102">
+        <v>3</v>
+      </c>
+      <c r="H45" s="103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="7">
         <v>5</v>
       </c>
-      <c r="C46" s="81" t="s">
+      <c r="C46" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="67" t="s">
+      <c r="D46" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="97">
+      <c r="E46" s="88">
         <v>4</v>
       </c>
-      <c r="G46" s="105"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G46" s="102">
+        <v>25</v>
+      </c>
+      <c r="H46" s="103"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="7">
         <v>6</v>
       </c>
-      <c r="C47" s="83"/>
-      <c r="D47" s="67" t="s">
+      <c r="C47" s="69"/>
+      <c r="D47" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="97">
+      <c r="E47" s="88">
         <v>4</v>
       </c>
-      <c r="G47" s="105"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G47" s="102">
+        <v>0</v>
+      </c>
+      <c r="H47" s="103">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="7">
         <v>7</v>
       </c>
-      <c r="C48" s="82"/>
-      <c r="D48" s="67" t="s">
+      <c r="C48" s="70"/>
+      <c r="D48" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="E48" s="97">
-        <v>1</v>
-      </c>
-      <c r="G48" s="105"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="88">
+        <v>1</v>
+      </c>
+      <c r="G48" s="102">
+        <v>0</v>
+      </c>
+      <c r="H48" s="103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="7">
         <v>8</v>
       </c>
-      <c r="C49" s="81" t="s">
+      <c r="C49" s="68" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="67" t="s">
+      <c r="D49" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="97">
+      <c r="E49" s="88">
         <v>2</v>
       </c>
-      <c r="G49" s="105"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G49" s="102">
+        <v>0</v>
+      </c>
+      <c r="H49" s="103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
         <v>9</v>
       </c>
-      <c r="C50" s="83"/>
-      <c r="D50" s="67" t="s">
+      <c r="C50" s="69"/>
+      <c r="D50" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E50" s="97">
+      <c r="E50" s="8">
         <v>2</v>
       </c>
-      <c r="G50" s="105"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G50" s="102">
+        <v>0</v>
+      </c>
+      <c r="H50" s="103"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="7">
         <v>10</v>
       </c>
-      <c r="C51" s="83"/>
-      <c r="D51" s="67" t="s">
+      <c r="C51" s="69"/>
+      <c r="D51" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="E51" s="97">
+      <c r="E51" s="88">
         <v>2</v>
       </c>
-      <c r="G51" s="105"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G51" s="102">
+        <v>8</v>
+      </c>
+      <c r="H51" s="103"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
         <v>11</v>
       </c>
-      <c r="C52" s="83"/>
-      <c r="D52" s="67" t="s">
+      <c r="C52" s="69"/>
+      <c r="D52" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="97">
+      <c r="E52" s="88">
         <v>2</v>
       </c>
-      <c r="G52" s="105"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G52" s="102">
+        <v>8</v>
+      </c>
+      <c r="H52" s="103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="7">
         <v>12</v>
       </c>
-      <c r="C53" s="82"/>
-      <c r="D53" s="1" t="s">
+      <c r="C53" s="70"/>
+      <c r="D53" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="E53" s="97">
+      <c r="E53" s="88">
         <v>2</v>
       </c>
-      <c r="G53" s="105"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G53" s="102">
+        <v>8</v>
+      </c>
+      <c r="H53" s="103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="7">
         <v>13</v>
       </c>
-      <c r="C54" s="81" t="s">
+      <c r="C54" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="D54" s="67" t="s">
+      <c r="D54" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E54" s="97">
+      <c r="E54" s="8">
         <v>3</v>
       </c>
-      <c r="G54" s="105"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G54" s="102"/>
+      <c r="H54" s="103"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="7">
         <v>14</v>
       </c>
-      <c r="C55" s="83"/>
-      <c r="D55" s="67" t="s">
+      <c r="C55" s="69"/>
+      <c r="D55" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E55" s="97">
-        <v>1</v>
-      </c>
-      <c r="G55" s="105"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E55" s="8">
+        <v>1</v>
+      </c>
+      <c r="G55" s="102"/>
+      <c r="H55" s="103"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="7">
         <v>15</v>
       </c>
-      <c r="C56" s="82"/>
-      <c r="D56" s="67" t="s">
+      <c r="C56" s="70"/>
+      <c r="D56" s="86" t="s">
         <v>114</v>
       </c>
-      <c r="E56" s="97">
-        <v>1</v>
-      </c>
-      <c r="G56" s="105"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E56" s="88">
+        <v>1</v>
+      </c>
+      <c r="G56" s="102"/>
+      <c r="H56" s="103"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="7">
         <v>16</v>
       </c>
-      <c r="C57" s="81" t="s">
+      <c r="C57" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="85" t="s">
+      <c r="D57" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="E57" s="98">
+      <c r="E57" s="99">
         <v>3</v>
       </c>
-      <c r="G57" s="105"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G57" s="102"/>
+      <c r="H57" s="103"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="7">
         <v>17</v>
       </c>
-      <c r="C58" s="84"/>
-      <c r="D58" s="87" t="s">
+      <c r="C58" s="71"/>
+      <c r="D58" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="E58" s="98">
+      <c r="E58" s="90">
         <v>4</v>
       </c>
-      <c r="G58" s="105"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G58" s="102">
+        <v>96</v>
+      </c>
+      <c r="H58" s="103"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="7">
         <v>18</v>
       </c>
-      <c r="C59" s="84"/>
-      <c r="D59" s="88" t="s">
+      <c r="C59" s="71"/>
+      <c r="D59" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="E59" s="99">
-        <v>1</v>
-      </c>
-      <c r="G59" s="105"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E59" s="108">
+        <v>1</v>
+      </c>
+      <c r="G59" s="102">
+        <v>4</v>
+      </c>
+      <c r="H59" s="103"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="7">
         <v>19</v>
       </c>
-      <c r="C60" s="84"/>
-      <c r="D60" s="88" t="s">
+      <c r="C60" s="71"/>
+      <c r="D60" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="100">
+      <c r="E60" s="93">
         <v>2</v>
       </c>
-      <c r="G60" s="105"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G60" s="102">
+        <v>23</v>
+      </c>
+      <c r="H60" s="103"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="7">
         <v>20</v>
       </c>
-      <c r="C61" s="84"/>
-      <c r="D61" s="88" t="s">
+      <c r="C61" s="71"/>
+      <c r="D61" s="92" t="s">
         <v>119</v>
       </c>
-      <c r="E61" s="100">
+      <c r="E61" s="93">
         <v>4</v>
       </c>
-      <c r="G61" s="105"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G61" s="102">
+        <v>21</v>
+      </c>
+      <c r="H61" s="103"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="7">
         <v>21</v>
       </c>
-      <c r="C62" s="84"/>
-      <c r="D62" s="88" t="s">
+      <c r="C62" s="71"/>
+      <c r="D62" s="92" t="s">
         <v>120</v>
       </c>
-      <c r="E62" s="100">
-        <v>1</v>
-      </c>
-      <c r="G62" s="105"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E62" s="93">
+        <v>1</v>
+      </c>
+      <c r="G62" s="102">
+        <v>24</v>
+      </c>
+      <c r="H62" s="103"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="7">
         <v>22</v>
       </c>
-      <c r="C63" s="84"/>
-      <c r="D63" s="88" t="s">
+      <c r="C63" s="71"/>
+      <c r="D63" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="E63" s="100">
+      <c r="E63" s="93">
         <v>21</v>
       </c>
-      <c r="G63" s="105"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G63" s="102">
+        <v>3</v>
+      </c>
+      <c r="H63" s="103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="7">
         <v>23</v>
       </c>
-      <c r="C64" s="84"/>
-      <c r="D64" s="88" t="s">
+      <c r="C64" s="71"/>
+      <c r="D64" s="92" t="s">
         <v>122</v>
       </c>
-      <c r="E64" s="100">
+      <c r="E64" s="93">
         <v>8</v>
       </c>
-      <c r="G64" s="105"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G64" s="102">
+        <v>16</v>
+      </c>
+      <c r="H64" s="103">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="7">
         <v>24</v>
       </c>
-      <c r="C65" s="84"/>
-      <c r="D65" s="88" t="s">
+      <c r="C65" s="71"/>
+      <c r="D65" s="92" t="s">
         <v>123</v>
       </c>
-      <c r="E65" s="100">
+      <c r="E65" s="93">
         <v>5</v>
       </c>
-      <c r="G65" s="105"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G65" s="102">
+        <v>20</v>
+      </c>
+      <c r="H65" s="103">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="7">
         <v>25</v>
       </c>
-      <c r="C66" s="84"/>
-      <c r="D66" s="89" t="s">
+      <c r="C66" s="71"/>
+      <c r="D66" s="94" t="s">
         <v>124</v>
       </c>
-      <c r="E66" s="101">
+      <c r="E66" s="95">
         <v>6</v>
       </c>
-      <c r="G66" s="105"/>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G66" s="102">
+        <v>13</v>
+      </c>
+      <c r="H66" s="103">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="7">
         <v>26</v>
       </c>
-      <c r="C67" s="83"/>
-      <c r="D67" s="90" t="s">
+      <c r="C67" s="69"/>
+      <c r="D67" s="109" t="s">
         <v>125</v>
       </c>
-      <c r="E67" s="100">
+      <c r="E67" s="108">
         <v>3</v>
       </c>
-      <c r="G67" s="105"/>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G67" s="102">
+        <v>5</v>
+      </c>
+      <c r="H67" s="103"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="7">
         <v>27</v>
       </c>
-      <c r="C68" s="84"/>
-      <c r="D68" s="85" t="s">
+      <c r="C68" s="71"/>
+      <c r="D68" s="89" t="s">
         <v>126</v>
       </c>
-      <c r="E68" s="55">
+      <c r="E68" s="90">
         <v>12</v>
       </c>
-      <c r="G68" s="105"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G68" s="102">
+        <v>9</v>
+      </c>
+      <c r="H68" s="103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="7">
         <v>28</v>
       </c>
-      <c r="C69" s="84"/>
-      <c r="D69" s="90" t="s">
+      <c r="C69" s="71"/>
+      <c r="D69" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="E69" s="100">
+      <c r="E69" s="93">
         <v>7</v>
       </c>
-      <c r="G69" s="105"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G69" s="102">
+        <v>14</v>
+      </c>
+      <c r="H69" s="103">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="7">
         <v>29</v>
       </c>
-      <c r="C70" s="84"/>
-      <c r="D70" s="90" t="s">
+      <c r="C70" s="71"/>
+      <c r="D70" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="E70" s="100">
+      <c r="E70" s="93">
         <v>10</v>
       </c>
-      <c r="G70" s="105"/>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G70" s="102">
+        <v>10</v>
+      </c>
+      <c r="H70" s="103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="7">
         <v>30</v>
       </c>
-      <c r="C71" s="84"/>
-      <c r="D71" s="90" t="s">
+      <c r="C71" s="71"/>
+      <c r="D71" s="96" t="s">
         <v>142</v>
       </c>
-      <c r="E71" s="100">
-        <v>1</v>
-      </c>
-      <c r="G71" s="105"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E71" s="93">
+        <v>2</v>
+      </c>
+      <c r="G71" s="102">
+        <v>18</v>
+      </c>
+      <c r="H71" s="103"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="7">
         <v>31</v>
       </c>
-      <c r="C72" s="84"/>
-      <c r="D72" s="90" t="s">
+      <c r="C72" s="71"/>
+      <c r="D72" s="96" t="s">
         <v>129</v>
       </c>
-      <c r="E72" s="100">
+      <c r="E72" s="93">
         <v>6</v>
       </c>
-      <c r="G72" s="105"/>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G72" s="102">
+        <v>14</v>
+      </c>
+      <c r="H72" s="103">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="7">
         <v>32</v>
       </c>
-      <c r="C73" s="84"/>
-      <c r="D73" s="90" t="s">
+      <c r="C73" s="71"/>
+      <c r="D73" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="E73" s="100">
+      <c r="E73" s="93">
         <v>4</v>
       </c>
-      <c r="G73" s="105"/>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G73" s="102">
+        <v>16</v>
+      </c>
+      <c r="H73" s="103">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="7">
         <v>33</v>
       </c>
-      <c r="C74" s="84"/>
-      <c r="D74" s="87" t="s">
+      <c r="C74" s="71"/>
+      <c r="D74" s="91" t="s">
         <v>132</v>
       </c>
-      <c r="E74" s="55">
+      <c r="E74" s="90">
         <v>2</v>
       </c>
-      <c r="G74" s="105"/>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G74" s="102">
+        <v>18</v>
+      </c>
+      <c r="H74" s="103"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="7">
         <v>34</v>
       </c>
-      <c r="C75" s="84"/>
-      <c r="D75" s="88" t="s">
+      <c r="C75" s="71"/>
+      <c r="D75" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="E75" s="100">
-        <v>1</v>
-      </c>
-      <c r="G75" s="105"/>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E75" s="93">
+        <v>1</v>
+      </c>
+      <c r="G75" s="102">
+        <v>19</v>
+      </c>
+      <c r="H75" s="103"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="7">
         <v>35</v>
       </c>
-      <c r="C76" s="84"/>
-      <c r="D76" s="88" t="s">
+      <c r="C76" s="71"/>
+      <c r="D76" s="92" t="s">
         <v>131</v>
       </c>
-      <c r="E76" s="100">
+      <c r="E76" s="93">
         <v>5</v>
       </c>
-      <c r="G76" s="105"/>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G76" s="102">
+        <v>15</v>
+      </c>
+      <c r="H76" s="103"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="7">
         <v>36</v>
       </c>
-      <c r="C77" s="84"/>
-      <c r="D77" s="88" t="s">
+      <c r="C77" s="71"/>
+      <c r="D77" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="E77" s="100">
+      <c r="E77" s="93">
         <v>2</v>
       </c>
-      <c r="G77" s="105"/>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G77" s="102">
+        <v>18</v>
+      </c>
+      <c r="H77" s="103"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="7">
         <v>37</v>
       </c>
-      <c r="C78" s="84"/>
-      <c r="D78" s="89" t="s">
+      <c r="C78" s="71"/>
+      <c r="D78" s="94" t="s">
         <v>135</v>
       </c>
-      <c r="E78" s="101">
+      <c r="E78" s="95">
         <v>2</v>
       </c>
-      <c r="G78" s="105"/>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G78" s="102">
+        <v>18</v>
+      </c>
+      <c r="H78" s="103"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="7">
         <v>38</v>
       </c>
-      <c r="C79" s="83"/>
-      <c r="D79" s="86" t="s">
+      <c r="C79" s="69"/>
+      <c r="D79" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="E79" s="101">
-        <v>1</v>
-      </c>
-      <c r="G79" s="105"/>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E79" s="95">
+        <v>1</v>
+      </c>
+      <c r="G79" s="102">
+        <v>9</v>
+      </c>
+      <c r="H79" s="103"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="7">
         <v>39</v>
       </c>
-      <c r="C80" s="82"/>
-      <c r="D80" s="67" t="s">
+      <c r="C80" s="70"/>
+      <c r="D80" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E80" s="8">
         <v>1</v>
       </c>
-      <c r="G80" s="105"/>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G80" s="102">
+        <v>2</v>
+      </c>
+      <c r="H80" s="103"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="7">
         <v>40</v>
       </c>
-      <c r="C81" s="81" t="s">
+      <c r="C81" s="68" t="s">
         <v>137</v>
       </c>
-      <c r="D81" s="67" t="s">
+      <c r="D81" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E81" s="8">
         <v>4</v>
       </c>
-      <c r="G81" s="105"/>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G81" s="102">
+        <v>7</v>
+      </c>
+      <c r="H81" s="103"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="7">
         <v>41</v>
       </c>
-      <c r="C82" s="82"/>
-      <c r="D82" s="67" t="s">
+      <c r="C82" s="70"/>
+      <c r="D82" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E82" s="8">
         <v>1</v>
       </c>
-      <c r="G82" s="105"/>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G82" s="102"/>
+      <c r="H82" s="103"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="7">
         <v>42</v>
       </c>
-      <c r="C83" s="81" t="s">
+      <c r="C83" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D83" s="67" t="s">
+      <c r="D83" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E83" s="8">
         <v>1</v>
       </c>
-      <c r="G83" s="105"/>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G83" s="102"/>
+      <c r="H83" s="103"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="7">
         <v>43</v>
       </c>
-      <c r="C84" s="83"/>
-      <c r="D84" s="67" t="s">
+      <c r="C84" s="69"/>
+      <c r="D84" s="1" t="s">
         <v>141</v>
       </c>
       <c r="E84" s="8">
         <v>1</v>
       </c>
-      <c r="G84" s="105"/>
-    </row>
-    <row r="85" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G84" s="102"/>
+      <c r="H84" s="103"/>
+    </row>
+    <row r="85" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="27">
         <v>44</v>
       </c>
-      <c r="C85" s="102"/>
-      <c r="D85" s="72" t="s">
+      <c r="C85" s="72"/>
+      <c r="D85" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="E85" s="103">
+      <c r="E85" s="67">
         <v>2</v>
       </c>
-      <c r="G85" s="107"/>
+      <c r="G85" s="104"/>
+      <c r="H85" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C49:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="C33:C36"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="L7:N7"/>
@@ -3117,6 +3280,16 @@
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="C49:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C85"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{009E80E0-CC73-4407-97F9-5CA562932134}"/>

</xml_diff>

<commit_message>
V0.3: Components File Update
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\SINDiB-MICROMOUSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A0CE99-59C6-4EEE-B213-E4DF6E902579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A03F8F-5873-4D10-BBBB-B89E6B20C923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
+    <workbookView xWindow="1620" yWindow="1395" windowWidth="21600" windowHeight="11295" xr2:uid="{0C7E4563-7DB7-41B6-8BF4-78D4DE27A5BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="149">
   <si>
     <t>COMPONENT</t>
   </si>
@@ -323,9 +323,6 @@
     <t>PCB - JLCPCB</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Biyon</t>
   </si>
   <si>
@@ -474,6 +471,21 @@
   </si>
   <si>
     <t>Expected Order</t>
+  </si>
+  <si>
+    <t>Alibaba Order</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Nushad</t>
+  </si>
+  <si>
+    <t>Mount</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -534,7 +546,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -615,12 +627,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -632,7 +638,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -912,30 +918,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1027,12 +1009,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1116,14 +1111,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
@@ -1137,7 +1126,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1145,28 +1133,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1175,6 +1196,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1186,50 +1213,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1558,8 +1541,8 @@
   </sheetPr>
   <dimension ref="B1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,17 +1562,17 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
       <c r="L2" s="29" t="s">
         <v>78</v>
       </c>
@@ -1635,7 +1618,7 @@
       <c r="B5" s="19">
         <v>1</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="105" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
@@ -1654,13 +1637,13 @@
       <c r="I5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="53"/>
+      <c r="J5" s="47"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="C6" s="79"/>
+      <c r="C6" s="103"/>
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
@@ -1683,7 +1666,7 @@
       <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="103" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1704,17 +1687,17 @@
         <v>79</v>
       </c>
       <c r="J7" s="36"/>
-      <c r="L7" s="80" t="s">
+      <c r="L7" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
+      <c r="M7" s="104"/>
+      <c r="N7" s="104"/>
     </row>
     <row r="8" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="103"/>
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1729,7 +1712,7 @@
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J8" s="36"/>
     </row>
@@ -1737,7 +1720,7 @@
       <c r="B9" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="79"/>
+      <c r="C9" s="103"/>
       <c r="D9" s="20" t="s">
         <v>10</v>
       </c>
@@ -1769,7 +1752,7 @@
       <c r="B10" s="7">
         <v>6</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1784,16 +1767,16 @@
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J10" s="36"/>
-      <c r="L10" s="46" t="s">
+      <c r="L10" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="M10" s="47" t="s">
+      <c r="M10" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="N10" s="48">
+      <c r="N10" s="89">
         <v>44809.72</v>
       </c>
     </row>
@@ -1801,7 +1784,7 @@
       <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="103" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1821,13 +1804,13 @@
         <v>15</v>
       </c>
       <c r="J11" s="26"/>
-      <c r="L11" s="49" t="s">
+      <c r="L11" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="50" t="s">
+      <c r="M11" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="N11" s="51">
+      <c r="N11" s="85">
         <v>7987.01</v>
       </c>
     </row>
@@ -1835,7 +1818,7 @@
       <c r="B12" s="7">
         <v>8</v>
       </c>
-      <c r="C12" s="79"/>
+      <c r="C12" s="103"/>
       <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1853,13 +1836,13 @@
         <v>16</v>
       </c>
       <c r="J12" s="26"/>
-      <c r="L12" s="49" t="s">
+      <c r="L12" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="50" t="s">
+      <c r="M12" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="N12" s="51">
+      <c r="N12" s="85">
         <v>10041.09</v>
       </c>
     </row>
@@ -1867,7 +1850,7 @@
       <c r="B13" s="7">
         <v>9</v>
       </c>
-      <c r="C13" s="79"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1885,13 +1868,13 @@
         <v>18</v>
       </c>
       <c r="J13" s="36"/>
-      <c r="L13" s="49" t="s">
+      <c r="L13" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="M13" s="50" t="s">
+      <c r="M13" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="51">
+      <c r="N13" s="85">
         <v>1228</v>
       </c>
     </row>
@@ -1899,7 +1882,7 @@
       <c r="B14" s="7">
         <v>10</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="103" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -1919,19 +1902,19 @@
         <v>69</v>
       </c>
       <c r="J14" s="26"/>
-      <c r="L14" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="M14" s="50" t="s">
+      <c r="L14" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="M14" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="N14" s="51">
+      <c r="N14" s="85">
         <v>4671.6899999999996</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
-      <c r="C15" s="79"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="37" t="s">
         <v>89</v>
       </c>
@@ -1949,13 +1932,13 @@
         <v>90</v>
       </c>
       <c r="J15" s="26"/>
-      <c r="L15" s="49" t="s">
+      <c r="L15" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M15" s="50" t="s">
+      <c r="M15" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="51">
+      <c r="N15" s="85">
         <v>939</v>
       </c>
     </row>
@@ -1963,7 +1946,7 @@
       <c r="B16" s="7">
         <v>11</v>
       </c>
-      <c r="C16" s="79"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="21" t="s">
         <v>70</v>
       </c>
@@ -1987,7 +1970,7 @@
       <c r="M16" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="N16" s="45">
+      <c r="N16" s="86">
         <v>-13709.74</v>
       </c>
     </row>
@@ -1995,7 +1978,7 @@
       <c r="B17" s="7">
         <v>12</v>
       </c>
-      <c r="C17" s="79"/>
+      <c r="C17" s="103"/>
       <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
@@ -2013,13 +1996,13 @@
         <v>34</v>
       </c>
       <c r="J17" s="36"/>
-      <c r="L17" s="49" t="s">
+      <c r="L17" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M17" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="N17" s="51">
+      <c r="M17" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="N17" s="85">
         <v>2138</v>
       </c>
     </row>
@@ -2027,7 +2010,7 @@
       <c r="B18" s="7">
         <v>13</v>
       </c>
-      <c r="C18" s="79"/>
+      <c r="C18" s="103"/>
       <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2045,22 +2028,22 @@
         <v>35</v>
       </c>
       <c r="J18" s="36"/>
-      <c r="L18" s="49" t="s">
+      <c r="L18" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="M18" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="N18" s="51">
+      <c r="M18" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="N18" s="85">
         <f>1685+180</f>
         <v>1865</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <v>14</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="103" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="21" t="s">
@@ -2080,22 +2063,22 @@
         <v>81</v>
       </c>
       <c r="J19" s="36"/>
-      <c r="L19" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="M19" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="N19" s="60">
+      <c r="L19" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="M19" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="N19" s="85">
         <f>240+190</f>
         <v>430</v>
       </c>
     </row>
-    <row r="20" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <v>15</v>
       </c>
-      <c r="C20" s="79"/>
+      <c r="C20" s="103"/>
       <c r="D20" s="21" t="s">
         <v>60</v>
       </c>
@@ -2113,20 +2096,21 @@
         <v>80</v>
       </c>
       <c r="J20" s="36"/>
-      <c r="L20" s="74" t="s">
-        <v>94</v>
-      </c>
-      <c r="M20" s="75"/>
-      <c r="N20" s="52">
-        <f>SUM(N10:N19)</f>
-        <v>60399.770000000011</v>
+      <c r="L20" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="N20" s="85">
+        <v>19765.439999999999</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <v>16</v>
       </c>
-      <c r="C21" s="79"/>
+      <c r="C21" s="103"/>
       <c r="D21" s="21" t="s">
         <v>59</v>
       </c>
@@ -2144,37 +2128,55 @@
         <v>68</v>
       </c>
       <c r="J21" s="26"/>
+      <c r="L21" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="M21" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="N21" s="85">
+        <v>1000</v>
+      </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <v>17</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="D22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="82">
+      <c r="E22" s="1">
         <v>6</v>
       </c>
-      <c r="F22" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="83"/>
-      <c r="H22" s="84">
+      <c r="F22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="32">
         <v>180</v>
       </c>
-      <c r="I22" s="82" t="s">
+      <c r="I22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J22" s="36"/>
+      <c r="L22" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="M22" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="N22" s="85">
+        <v>1000</v>
+      </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <v>18</v>
       </c>
-      <c r="C23" s="79"/>
+      <c r="C23" s="103"/>
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2192,12 +2194,15 @@
         <v>43</v>
       </c>
       <c r="J23" s="36"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="8"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <v>19</v>
       </c>
-      <c r="C24" s="79"/>
+      <c r="C24" s="103"/>
       <c r="D24" s="21" t="s">
         <v>28</v>
       </c>
@@ -2215,12 +2220,15 @@
         <v>44</v>
       </c>
       <c r="J24" s="36"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="7"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="7">
         <v>20</v>
       </c>
-      <c r="C25" s="79"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="1" t="s">
         <v>27</v>
       </c>
@@ -2238,12 +2246,15 @@
         <v>65</v>
       </c>
       <c r="J25" s="36"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L25" s="91"/>
+      <c r="M25" s="74"/>
+      <c r="N25" s="75"/>
+    </row>
+    <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
         <v>21</v>
       </c>
-      <c r="C26" s="79"/>
+      <c r="C26" s="103"/>
       <c r="D26" s="21" t="s">
         <v>32</v>
       </c>
@@ -2261,12 +2272,20 @@
         <v>31</v>
       </c>
       <c r="J26" s="36"/>
+      <c r="L26" s="100" t="s">
+        <v>148</v>
+      </c>
+      <c r="M26" s="101"/>
+      <c r="N26" s="90">
+        <f>SUM(N10:N25)</f>
+        <v>82165.210000000006</v>
+      </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
         <v>22</v>
       </c>
-      <c r="C27" s="79"/>
+      <c r="C27" s="103"/>
       <c r="D27" s="1" t="s">
         <v>45</v>
       </c>
@@ -2289,7 +2308,7 @@
       <c r="B28" s="7">
         <v>23</v>
       </c>
-      <c r="C28" s="79"/>
+      <c r="C28" s="103"/>
       <c r="D28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2312,7 +2331,7 @@
       <c r="B29" s="7">
         <v>24</v>
       </c>
-      <c r="C29" s="79"/>
+      <c r="C29" s="103"/>
       <c r="D29" s="21" t="s">
         <v>66</v>
       </c>
@@ -2335,7 +2354,7 @@
       <c r="B30" s="7">
         <v>25</v>
       </c>
-      <c r="C30" s="79"/>
+      <c r="C30" s="103"/>
       <c r="D30" s="21" t="s">
         <v>56</v>
       </c>
@@ -2358,7 +2377,7 @@
       <c r="B31" s="7">
         <v>26</v>
       </c>
-      <c r="C31" s="79" t="s">
+      <c r="C31" s="103" t="s">
         <v>55</v>
       </c>
       <c r="D31" s="20" t="s">
@@ -2383,7 +2402,7 @@
       <c r="B32" s="7">
         <v>27</v>
       </c>
-      <c r="C32" s="79"/>
+      <c r="C32" s="103"/>
       <c r="D32" s="16" t="s">
         <v>57</v>
       </c>
@@ -2406,21 +2425,21 @@
       <c r="B33" s="7">
         <v>28</v>
       </c>
-      <c r="C33" s="76" t="s">
+      <c r="C33" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="54" t="s">
+      <c r="D33" s="48" t="s">
         <v>73</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="32"/>
-      <c r="I33" s="55" t="s">
+      <c r="I33" s="49" t="s">
         <v>76</v>
       </c>
       <c r="J33" s="36"/>
@@ -2429,21 +2448,21 @@
       <c r="B34" s="7">
         <v>29</v>
       </c>
-      <c r="C34" s="76"/>
+      <c r="C34" s="98"/>
       <c r="D34" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="55" t="s">
+      <c r="F34" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="G34" s="56"/>
+      <c r="G34" s="50"/>
       <c r="H34" s="32">
         <v>160</v>
       </c>
-      <c r="I34" s="55" t="s">
+      <c r="I34" s="49" t="s">
         <v>76</v>
       </c>
       <c r="J34" s="36"/>
@@ -2452,21 +2471,21 @@
       <c r="B35" s="7">
         <v>30</v>
       </c>
-      <c r="C35" s="76"/>
+      <c r="C35" s="98"/>
       <c r="D35" s="1" t="s">
         <v>75</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
       </c>
-      <c r="F35" s="55" t="s">
+      <c r="F35" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="G35" s="56"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="32">
         <v>1375</v>
       </c>
-      <c r="I35" s="55" t="s">
+      <c r="I35" s="49" t="s">
         <v>76</v>
       </c>
       <c r="J35" s="36"/>
@@ -2475,35 +2494,35 @@
       <c r="B36" s="27">
         <v>31</v>
       </c>
-      <c r="C36" s="77"/>
-      <c r="D36" s="57" t="s">
+      <c r="C36" s="99"/>
+      <c r="D36" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="51">
+        <v>1</v>
+      </c>
+      <c r="F36" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53">
+        <v>175</v>
+      </c>
+      <c r="I36" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="57">
-        <v>1</v>
-      </c>
-      <c r="F36" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="G36" s="58"/>
-      <c r="H36" s="59">
-        <v>175</v>
-      </c>
-      <c r="I36" s="57" t="s">
-        <v>100</v>
-      </c>
-      <c r="J36" s="61"/>
+      <c r="J36" s="54"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G38"/>
       <c r="H38"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C39" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
+      <c r="C39" s="97" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="97"/>
+      <c r="E39" s="97"/>
       <c r="G39"/>
       <c r="H39"/>
     </row>
@@ -2512,40 +2531,40 @@
       <c r="H40"/>
     </row>
     <row r="41" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="62"/>
-      <c r="C41" s="63" t="s">
+      <c r="B41" s="55"/>
+      <c r="C41" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="63" t="s">
+      <c r="D41" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="G41" s="100" t="s">
+      <c r="G41" s="76" t="s">
+        <v>142</v>
+      </c>
+      <c r="H41" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="H41" s="101" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="65">
-        <v>1</v>
-      </c>
-      <c r="C42" s="66" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42" s="85" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" s="87">
-        <v>1</v>
-      </c>
-      <c r="G42" s="65">
-        <v>1</v>
-      </c>
-      <c r="H42" s="110">
+      <c r="B42" s="58">
+        <v>1</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="63">
+        <v>1</v>
+      </c>
+      <c r="G42" s="58">
+        <v>1</v>
+      </c>
+      <c r="H42" s="84">
         <v>5</v>
       </c>
     </row>
@@ -2553,19 +2572,19 @@
       <c r="B43" s="7">
         <v>2</v>
       </c>
-      <c r="C43" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="D43" s="86" t="s">
+      <c r="C43" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="88">
-        <v>1</v>
-      </c>
-      <c r="G43" s="102">
+      <c r="E43" s="64">
+        <v>1</v>
+      </c>
+      <c r="G43" s="77">
         <v>3</v>
       </c>
-      <c r="H43" s="111">
+      <c r="H43" s="78">
         <v>5</v>
       </c>
     </row>
@@ -2573,17 +2592,17 @@
       <c r="B44" s="7">
         <v>3</v>
       </c>
-      <c r="C44" s="69"/>
-      <c r="D44" s="82" t="s">
+      <c r="C44" s="93"/>
+      <c r="D44" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="106">
-        <v>1</v>
-      </c>
-      <c r="G44" s="102">
+      <c r="E44" s="8">
+        <v>1</v>
+      </c>
+      <c r="G44" s="77">
         <v>3</v>
       </c>
-      <c r="H44" s="111">
+      <c r="H44" s="78">
         <v>5</v>
       </c>
     </row>
@@ -2591,17 +2610,17 @@
       <c r="B45" s="7">
         <v>4</v>
       </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="86" t="s">
+      <c r="C45" s="94"/>
+      <c r="D45" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="88">
-        <v>1</v>
-      </c>
-      <c r="G45" s="102">
+      <c r="E45" s="64">
+        <v>1</v>
+      </c>
+      <c r="G45" s="77">
         <v>3</v>
       </c>
-      <c r="H45" s="103">
+      <c r="H45" s="78">
         <v>5</v>
       </c>
     </row>
@@ -2609,35 +2628,35 @@
       <c r="B46" s="7">
         <v>5</v>
       </c>
-      <c r="C46" s="68" t="s">
-        <v>112</v>
-      </c>
-      <c r="D46" s="86" t="s">
+      <c r="C46" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="D46" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="88">
+      <c r="E46" s="64">
         <v>4</v>
       </c>
-      <c r="G46" s="102">
+      <c r="G46" s="77">
         <v>25</v>
       </c>
-      <c r="H46" s="103"/>
+      <c r="H46" s="78"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="7">
         <v>6</v>
       </c>
-      <c r="C47" s="69"/>
-      <c r="D47" s="86" t="s">
+      <c r="C47" s="93"/>
+      <c r="D47" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="88">
+      <c r="E47" s="64">
         <v>4</v>
       </c>
-      <c r="G47" s="102">
+      <c r="G47" s="77">
         <v>0</v>
       </c>
-      <c r="H47" s="103">
+      <c r="H47" s="78">
         <v>30</v>
       </c>
     </row>
@@ -2645,17 +2664,17 @@
       <c r="B48" s="7">
         <v>7</v>
       </c>
-      <c r="C48" s="70"/>
-      <c r="D48" s="86" t="s">
+      <c r="C48" s="94"/>
+      <c r="D48" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="E48" s="88">
-        <v>1</v>
-      </c>
-      <c r="G48" s="102">
+      <c r="E48" s="64">
+        <v>1</v>
+      </c>
+      <c r="G48" s="77">
         <v>0</v>
       </c>
-      <c r="H48" s="103">
+      <c r="H48" s="78">
         <v>5</v>
       </c>
     </row>
@@ -2663,19 +2682,19 @@
       <c r="B49" s="7">
         <v>8</v>
       </c>
-      <c r="C49" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="D49" s="86" t="s">
-        <v>108</v>
-      </c>
-      <c r="E49" s="88">
+      <c r="C49" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="64">
         <v>2</v>
       </c>
-      <c r="G49" s="102">
+      <c r="G49" s="77">
         <v>0</v>
       </c>
-      <c r="H49" s="103">
+      <c r="H49" s="78">
         <v>8</v>
       </c>
     </row>
@@ -2683,49 +2702,49 @@
       <c r="B50" s="7">
         <v>9</v>
       </c>
-      <c r="C50" s="69"/>
+      <c r="C50" s="93"/>
       <c r="D50" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E50" s="8">
         <v>2</v>
       </c>
-      <c r="G50" s="102">
+      <c r="G50" s="77">
         <v>0</v>
       </c>
-      <c r="H50" s="103"/>
+      <c r="H50" s="78"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="7">
         <v>10</v>
       </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="86" t="s">
-        <v>110</v>
-      </c>
-      <c r="E51" s="88">
+      <c r="C51" s="93"/>
+      <c r="D51" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="64">
         <v>2</v>
       </c>
-      <c r="G51" s="102">
+      <c r="G51" s="77">
         <v>8</v>
       </c>
-      <c r="H51" s="103"/>
+      <c r="H51" s="78"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
         <v>11</v>
       </c>
-      <c r="C52" s="69"/>
-      <c r="D52" s="86" t="s">
+      <c r="C52" s="93"/>
+      <c r="D52" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="E52" s="88">
+      <c r="E52" s="64">
         <v>2</v>
       </c>
-      <c r="G52" s="102">
+      <c r="G52" s="77">
         <v>8</v>
       </c>
-      <c r="H52" s="103">
+      <c r="H52" s="78">
         <v>10</v>
       </c>
     </row>
@@ -2733,17 +2752,17 @@
       <c r="B53" s="7">
         <v>12</v>
       </c>
-      <c r="C53" s="70"/>
-      <c r="D53" s="86" t="s">
+      <c r="C53" s="94"/>
+      <c r="D53" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E53" s="88">
+      <c r="E53" s="64">
         <v>2</v>
       </c>
-      <c r="G53" s="102">
+      <c r="G53" s="77">
         <v>8</v>
       </c>
-      <c r="H53" s="103">
+      <c r="H53" s="78">
         <v>10</v>
       </c>
     </row>
@@ -2751,7 +2770,7 @@
       <c r="B54" s="7">
         <v>13</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="C54" s="92" t="s">
         <v>58</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2760,148 +2779,148 @@
       <c r="E54" s="8">
         <v>3</v>
       </c>
-      <c r="G54" s="102"/>
-      <c r="H54" s="103"/>
+      <c r="G54" s="77"/>
+      <c r="H54" s="78"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="7">
         <v>14</v>
       </c>
-      <c r="C55" s="69"/>
+      <c r="C55" s="93"/>
       <c r="D55" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E55" s="8">
         <v>1</v>
       </c>
-      <c r="G55" s="102"/>
-      <c r="H55" s="103"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="78"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="7">
         <v>15</v>
       </c>
-      <c r="C56" s="70"/>
-      <c r="D56" s="86" t="s">
-        <v>114</v>
-      </c>
-      <c r="E56" s="88">
-        <v>1</v>
-      </c>
-      <c r="G56" s="102"/>
-      <c r="H56" s="103"/>
+      <c r="C56" s="94"/>
+      <c r="D56" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="E56" s="64">
+        <v>1</v>
+      </c>
+      <c r="G56" s="77"/>
+      <c r="H56" s="78"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="7">
         <v>16</v>
       </c>
-      <c r="C57" s="68" t="s">
-        <v>138</v>
-      </c>
-      <c r="D57" s="98" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="99">
+      <c r="C57" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" s="75">
         <v>3</v>
       </c>
-      <c r="G57" s="102"/>
-      <c r="H57" s="103"/>
+      <c r="G57" s="77"/>
+      <c r="H57" s="78"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="7">
         <v>17</v>
       </c>
-      <c r="C58" s="71"/>
-      <c r="D58" s="91" t="s">
-        <v>116</v>
-      </c>
-      <c r="E58" s="90">
+      <c r="C58" s="95"/>
+      <c r="D58" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="E58" s="66">
         <v>4</v>
       </c>
-      <c r="G58" s="102">
+      <c r="G58" s="77">
         <v>96</v>
       </c>
-      <c r="H58" s="103"/>
+      <c r="H58" s="78"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="7">
         <v>18</v>
       </c>
-      <c r="C59" s="71"/>
-      <c r="D59" s="107" t="s">
-        <v>117</v>
-      </c>
-      <c r="E59" s="108">
-        <v>1</v>
-      </c>
-      <c r="G59" s="102">
+      <c r="C59" s="95"/>
+      <c r="D59" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="E59" s="82">
+        <v>1</v>
+      </c>
+      <c r="G59" s="77">
         <v>4</v>
       </c>
-      <c r="H59" s="103"/>
+      <c r="H59" s="78"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="7">
         <v>19</v>
       </c>
-      <c r="C60" s="71"/>
-      <c r="D60" s="92" t="s">
-        <v>118</v>
-      </c>
-      <c r="E60" s="93">
+      <c r="C60" s="95"/>
+      <c r="D60" s="68" t="s">
+        <v>117</v>
+      </c>
+      <c r="E60" s="69">
         <v>2</v>
       </c>
-      <c r="G60" s="102">
+      <c r="G60" s="77">
         <v>23</v>
       </c>
-      <c r="H60" s="103"/>
+      <c r="H60" s="78"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="7">
         <v>20</v>
       </c>
-      <c r="C61" s="71"/>
-      <c r="D61" s="92" t="s">
-        <v>119</v>
-      </c>
-      <c r="E61" s="93">
+      <c r="C61" s="95"/>
+      <c r="D61" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" s="69">
         <v>4</v>
       </c>
-      <c r="G61" s="102">
+      <c r="G61" s="77">
         <v>21</v>
       </c>
-      <c r="H61" s="103"/>
+      <c r="H61" s="78"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="7">
         <v>21</v>
       </c>
-      <c r="C62" s="71"/>
-      <c r="D62" s="92" t="s">
-        <v>120</v>
-      </c>
-      <c r="E62" s="93">
-        <v>1</v>
-      </c>
-      <c r="G62" s="102">
+      <c r="C62" s="95"/>
+      <c r="D62" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="E62" s="69">
+        <v>1</v>
+      </c>
+      <c r="G62" s="77">
         <v>24</v>
       </c>
-      <c r="H62" s="103"/>
+      <c r="H62" s="78"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="7">
         <v>22</v>
       </c>
-      <c r="C63" s="71"/>
-      <c r="D63" s="92" t="s">
-        <v>121</v>
-      </c>
-      <c r="E63" s="93">
+      <c r="C63" s="95"/>
+      <c r="D63" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="E63" s="69">
         <v>21</v>
       </c>
-      <c r="G63" s="102">
+      <c r="G63" s="77">
         <v>3</v>
       </c>
-      <c r="H63" s="103">
+      <c r="H63" s="78">
         <v>100</v>
       </c>
     </row>
@@ -2909,17 +2928,17 @@
       <c r="B64" s="7">
         <v>23</v>
       </c>
-      <c r="C64" s="71"/>
-      <c r="D64" s="92" t="s">
-        <v>122</v>
-      </c>
-      <c r="E64" s="93">
+      <c r="C64" s="95"/>
+      <c r="D64" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" s="69">
         <v>8</v>
       </c>
-      <c r="G64" s="102">
+      <c r="G64" s="77">
         <v>16</v>
       </c>
-      <c r="H64" s="103">
+      <c r="H64" s="78">
         <v>50</v>
       </c>
     </row>
@@ -2927,17 +2946,17 @@
       <c r="B65" s="7">
         <v>24</v>
       </c>
-      <c r="C65" s="71"/>
-      <c r="D65" s="92" t="s">
-        <v>123</v>
-      </c>
-      <c r="E65" s="93">
+      <c r="C65" s="95"/>
+      <c r="D65" s="68" t="s">
+        <v>122</v>
+      </c>
+      <c r="E65" s="69">
         <v>5</v>
       </c>
-      <c r="G65" s="102">
+      <c r="G65" s="77">
         <v>20</v>
       </c>
-      <c r="H65" s="103">
+      <c r="H65" s="78">
         <v>25</v>
       </c>
     </row>
@@ -2945,17 +2964,17 @@
       <c r="B66" s="7">
         <v>25</v>
       </c>
-      <c r="C66" s="71"/>
-      <c r="D66" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="E66" s="95">
+      <c r="C66" s="95"/>
+      <c r="D66" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="E66" s="71">
         <v>6</v>
       </c>
-      <c r="G66" s="102">
+      <c r="G66" s="77">
         <v>13</v>
       </c>
-      <c r="H66" s="103">
+      <c r="H66" s="78">
         <v>50</v>
       </c>
     </row>
@@ -2963,33 +2982,33 @@
       <c r="B67" s="7">
         <v>26</v>
       </c>
-      <c r="C67" s="69"/>
-      <c r="D67" s="109" t="s">
-        <v>125</v>
-      </c>
-      <c r="E67" s="108">
+      <c r="C67" s="93"/>
+      <c r="D67" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="E67" s="82">
         <v>3</v>
       </c>
-      <c r="G67" s="102">
+      <c r="G67" s="77">
         <v>5</v>
       </c>
-      <c r="H67" s="103"/>
+      <c r="H67" s="78"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="7">
         <v>27</v>
       </c>
-      <c r="C68" s="71"/>
-      <c r="D68" s="89" t="s">
-        <v>126</v>
-      </c>
-      <c r="E68" s="90">
+      <c r="C68" s="95"/>
+      <c r="D68" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="E68" s="66">
         <v>12</v>
       </c>
-      <c r="G68" s="102">
+      <c r="G68" s="77">
         <v>9</v>
       </c>
-      <c r="H68" s="103">
+      <c r="H68" s="78">
         <v>100</v>
       </c>
     </row>
@@ -2997,17 +3016,17 @@
       <c r="B69" s="7">
         <v>28</v>
       </c>
-      <c r="C69" s="71"/>
-      <c r="D69" s="96" t="s">
-        <v>127</v>
-      </c>
-      <c r="E69" s="93">
+      <c r="C69" s="95"/>
+      <c r="D69" s="72" t="s">
+        <v>126</v>
+      </c>
+      <c r="E69" s="69">
         <v>7</v>
       </c>
-      <c r="G69" s="102">
+      <c r="G69" s="77">
         <v>14</v>
       </c>
-      <c r="H69" s="103">
+      <c r="H69" s="78">
         <v>50</v>
       </c>
     </row>
@@ -3015,17 +3034,17 @@
       <c r="B70" s="7">
         <v>29</v>
       </c>
-      <c r="C70" s="71"/>
-      <c r="D70" s="96" t="s">
-        <v>128</v>
-      </c>
-      <c r="E70" s="93">
+      <c r="C70" s="95"/>
+      <c r="D70" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E70" s="69">
         <v>10</v>
       </c>
-      <c r="G70" s="102">
+      <c r="G70" s="77">
         <v>10</v>
       </c>
-      <c r="H70" s="103">
+      <c r="H70" s="78">
         <v>100</v>
       </c>
     </row>
@@ -3033,33 +3052,33 @@
       <c r="B71" s="7">
         <v>30</v>
       </c>
-      <c r="C71" s="71"/>
-      <c r="D71" s="96" t="s">
-        <v>142</v>
-      </c>
-      <c r="E71" s="93">
+      <c r="C71" s="95"/>
+      <c r="D71" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="E71" s="69">
         <v>2</v>
       </c>
-      <c r="G71" s="102">
+      <c r="G71" s="77">
         <v>18</v>
       </c>
-      <c r="H71" s="103"/>
+      <c r="H71" s="78"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="7">
         <v>31</v>
       </c>
-      <c r="C72" s="71"/>
-      <c r="D72" s="96" t="s">
-        <v>129</v>
-      </c>
-      <c r="E72" s="93">
+      <c r="C72" s="95"/>
+      <c r="D72" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="E72" s="69">
         <v>6</v>
       </c>
-      <c r="G72" s="102">
+      <c r="G72" s="77">
         <v>14</v>
       </c>
-      <c r="H72" s="103">
+      <c r="H72" s="78">
         <v>50</v>
       </c>
     </row>
@@ -3067,17 +3086,17 @@
       <c r="B73" s="7">
         <v>32</v>
       </c>
-      <c r="C73" s="71"/>
-      <c r="D73" s="96" t="s">
-        <v>130</v>
-      </c>
-      <c r="E73" s="93">
+      <c r="C73" s="95"/>
+      <c r="D73" s="72" t="s">
+        <v>129</v>
+      </c>
+      <c r="E73" s="69">
         <v>4</v>
       </c>
-      <c r="G73" s="102">
+      <c r="G73" s="77">
         <v>16</v>
       </c>
-      <c r="H73" s="103">
+      <c r="H73" s="78">
         <v>50</v>
       </c>
     </row>
@@ -3085,120 +3104,120 @@
       <c r="B74" s="7">
         <v>33</v>
       </c>
-      <c r="C74" s="71"/>
-      <c r="D74" s="91" t="s">
-        <v>132</v>
-      </c>
-      <c r="E74" s="90">
+      <c r="C74" s="95"/>
+      <c r="D74" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="E74" s="66">
         <v>2</v>
       </c>
-      <c r="G74" s="102">
+      <c r="G74" s="77">
         <v>18</v>
       </c>
-      <c r="H74" s="103"/>
+      <c r="H74" s="78"/>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="7">
         <v>34</v>
       </c>
-      <c r="C75" s="71"/>
-      <c r="D75" s="92" t="s">
-        <v>133</v>
-      </c>
-      <c r="E75" s="93">
-        <v>1</v>
-      </c>
-      <c r="G75" s="102">
+      <c r="C75" s="95"/>
+      <c r="D75" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="E75" s="69">
+        <v>1</v>
+      </c>
+      <c r="G75" s="77">
         <v>19</v>
       </c>
-      <c r="H75" s="103"/>
+      <c r="H75" s="78"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="7">
         <v>35</v>
       </c>
-      <c r="C76" s="71"/>
-      <c r="D76" s="92" t="s">
-        <v>131</v>
-      </c>
-      <c r="E76" s="93">
+      <c r="C76" s="95"/>
+      <c r="D76" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="E76" s="69">
         <v>5</v>
       </c>
-      <c r="G76" s="102">
+      <c r="G76" s="77">
         <v>15</v>
       </c>
-      <c r="H76" s="103"/>
+      <c r="H76" s="78"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="7">
         <v>36</v>
       </c>
-      <c r="C77" s="71"/>
-      <c r="D77" s="92" t="s">
-        <v>134</v>
-      </c>
-      <c r="E77" s="93">
+      <c r="C77" s="95"/>
+      <c r="D77" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="E77" s="69">
         <v>2</v>
       </c>
-      <c r="G77" s="102">
+      <c r="G77" s="77">
         <v>18</v>
       </c>
-      <c r="H77" s="103"/>
+      <c r="H77" s="78"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="7">
         <v>37</v>
       </c>
-      <c r="C78" s="71"/>
-      <c r="D78" s="94" t="s">
-        <v>135</v>
-      </c>
-      <c r="E78" s="95">
+      <c r="C78" s="95"/>
+      <c r="D78" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" s="71">
         <v>2</v>
       </c>
-      <c r="G78" s="102">
+      <c r="G78" s="77">
         <v>18</v>
       </c>
-      <c r="H78" s="103"/>
+      <c r="H78" s="78"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="7">
         <v>38</v>
       </c>
-      <c r="C79" s="69"/>
-      <c r="D79" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="E79" s="95">
-        <v>1</v>
-      </c>
-      <c r="G79" s="102">
+      <c r="C79" s="93"/>
+      <c r="D79" s="73" t="s">
+        <v>135</v>
+      </c>
+      <c r="E79" s="71">
+        <v>1</v>
+      </c>
+      <c r="G79" s="77">
         <v>9</v>
       </c>
-      <c r="H79" s="103"/>
+      <c r="H79" s="78"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="7">
         <v>39</v>
       </c>
-      <c r="C80" s="70"/>
+      <c r="C80" s="94"/>
       <c r="D80" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E80" s="8">
         <v>1</v>
       </c>
-      <c r="G80" s="102">
+      <c r="G80" s="77">
         <v>2</v>
       </c>
-      <c r="H80" s="103"/>
+      <c r="H80" s="78"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="7">
         <v>40</v>
       </c>
-      <c r="C81" s="68" t="s">
-        <v>137</v>
+      <c r="C81" s="92" t="s">
+        <v>136</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>53</v>
@@ -3206,68 +3225,68 @@
       <c r="E81" s="8">
         <v>4</v>
       </c>
-      <c r="G81" s="102">
+      <c r="G81" s="77">
         <v>7</v>
       </c>
-      <c r="H81" s="103"/>
+      <c r="H81" s="78"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="7">
         <v>41</v>
       </c>
-      <c r="C82" s="70"/>
+      <c r="C82" s="94"/>
       <c r="D82" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E82" s="8">
         <v>1</v>
       </c>
-      <c r="G82" s="102"/>
-      <c r="H82" s="103"/>
+      <c r="G82" s="77"/>
+      <c r="H82" s="78"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="7">
         <v>42</v>
       </c>
-      <c r="C83" s="68" t="s">
+      <c r="C83" s="92" t="s">
         <v>26</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E83" s="8">
         <v>1</v>
       </c>
-      <c r="G83" s="102"/>
-      <c r="H83" s="103"/>
+      <c r="G83" s="77"/>
+      <c r="H83" s="78"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="7">
         <v>43</v>
       </c>
-      <c r="C84" s="69"/>
+      <c r="C84" s="93"/>
       <c r="D84" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E84" s="8">
         <v>1</v>
       </c>
-      <c r="G84" s="102"/>
-      <c r="H84" s="103"/>
+      <c r="G84" s="77"/>
+      <c r="H84" s="78"/>
     </row>
     <row r="85" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="27">
         <v>44</v>
       </c>
-      <c r="C85" s="72"/>
-      <c r="D85" s="57" t="s">
-        <v>140</v>
-      </c>
-      <c r="E85" s="67">
+      <c r="C85" s="96"/>
+      <c r="D85" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="E85" s="60">
         <v>2</v>
       </c>
-      <c r="G85" s="104"/>
-      <c r="H85" s="105"/>
+      <c r="G85" s="79"/>
+      <c r="H85" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -3283,8 +3302,8 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="C46:C48"/>
-    <mergeCell ref="L20:M20"/>
     <mergeCell ref="C33:C36"/>
+    <mergeCell ref="L26:M26"/>
     <mergeCell ref="C49:C53"/>
     <mergeCell ref="C54:C56"/>
     <mergeCell ref="C57:C80"/>

</xml_diff>